<commit_message>
Leads Creation and Convert
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SalesForceAutomation\SalesforceAutomation\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B6FE56-912C-4BEB-B755-7BB9B2A4C039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11440" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WebTestData" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="115">
   <si>
     <t>TestData</t>
   </si>
@@ -349,19 +354,31 @@
   </si>
   <si>
     <t>demo@yahooo.com</t>
+  </si>
+  <si>
+    <t>CityName</t>
+  </si>
+  <si>
+    <t>Anil</t>
+  </si>
+  <si>
+    <t>anil53756@gmail.com</t>
+  </si>
+  <si>
+    <t>https://testingxperts61-dev-ed.develop.my.salesforce.com</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Sharma@123#&amp;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -396,154 +413,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -568,194 +443,8 @@
         <bgColor rgb="FF95B3D7"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -795,11 +484,33 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -810,329 +521,42 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="48" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1205,6 +629,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1462,42 +889,42 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="G2 F10 A1"/>
+      <selection sqref="G2 F10 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.859375" customWidth="1"/>
-    <col min="2" max="3" width="15.2890625" customWidth="1"/>
-    <col min="4" max="4" width="27.421875" customWidth="1"/>
-    <col min="5" max="5" width="9.421875" customWidth="1"/>
-    <col min="6" max="6" width="10.8515625" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" customWidth="1"/>
-    <col min="8" max="8" width="26.2890625" customWidth="1"/>
-    <col min="9" max="9" width="10.1328125" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="13" width="8.671875" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" customWidth="1"/>
-    <col min="15" max="15" width="21.140625" customWidth="1"/>
-    <col min="16" max="16" width="8.671875" customWidth="1"/>
-    <col min="17" max="17" width="12.2890625" customWidth="1"/>
-    <col min="18" max="18" width="26.2890625" customWidth="1"/>
-    <col min="19" max="19" width="19.7109375" customWidth="1"/>
-    <col min="20" max="20" width="15.5703125" customWidth="1"/>
-    <col min="21" max="21" width="14.859375" customWidth="1"/>
-    <col min="22" max="22" width="18.7109375" customWidth="1"/>
-    <col min="23" max="23" width="21.140625" customWidth="1"/>
-    <col min="24" max="24" width="32.2890625" customWidth="1"/>
-    <col min="25" max="1025" width="8.671875" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" customWidth="1"/>
+    <col min="7" max="7" width="28.1796875" customWidth="1"/>
+    <col min="8" max="8" width="26.26953125" customWidth="1"/>
+    <col min="9" max="9" width="10.08984375" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" customWidth="1"/>
+    <col min="11" max="13" width="8.6328125" customWidth="1"/>
+    <col min="14" max="14" width="12.7265625" customWidth="1"/>
+    <col min="15" max="15" width="21.1796875" customWidth="1"/>
+    <col min="16" max="16" width="8.6328125" customWidth="1"/>
+    <col min="17" max="17" width="12.26953125" customWidth="1"/>
+    <col min="18" max="18" width="26.26953125" customWidth="1"/>
+    <col min="19" max="19" width="19.7265625" customWidth="1"/>
+    <col min="20" max="20" width="15.54296875" customWidth="1"/>
+    <col min="21" max="21" width="14.81640625" customWidth="1"/>
+    <col min="22" max="22" width="18.7265625" customWidth="1"/>
+    <col min="23" max="23" width="21.1796875" customWidth="1"/>
+    <col min="24" max="24" width="32.26953125" customWidth="1"/>
+    <col min="25" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -1587,7 +1014,7 @@
       <c r="D2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1661,7 +1088,7 @@
       <c r="D3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1713,30 +1140,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="G2 F10 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.421875" customWidth="1"/>
-    <col min="3" max="3" width="32.2890625" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="7" width="8.671875" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="1025" width="8.671875" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="32.26953125" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1"/>
+    <col min="5" max="7" width="8.6328125" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" customWidth="1"/>
+    <col min="9" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1765,84 +1190,82 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" ht="14.8" spans="1:8">
+    <row r="2" spans="1:8" ht="15.5">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="9">
         <v>9888882626</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" ht="14.8" spans="1:8">
+    <row r="3" spans="1:8" ht="15.5">
       <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="9">
         <v>9888882626</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="10" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="w@maxbupa.com"/>
-    <hyperlink ref="H3" r:id="rId1" display="w@maxbupa.com"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="G2 F10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.2890625" customWidth="1"/>
-    <col min="2" max="2" width="27.578125" customWidth="1"/>
-    <col min="3" max="3" width="12.421875" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.671875" customWidth="1"/>
-    <col min="7" max="7" width="45.5703125" customWidth="1"/>
-    <col min="8" max="1025" width="8.671875" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" customWidth="1"/>
+    <col min="2" max="2" width="27.54296875" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" customWidth="1"/>
+    <col min="5" max="5" width="29.7265625" customWidth="1"/>
+    <col min="6" max="6" width="8.6328125" customWidth="1"/>
+    <col min="7" max="7" width="45.54296875" customWidth="1"/>
+    <col min="8" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1872,7 +1295,7 @@
       <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1881,7 +1304,7 @@
       <c r="D2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="3" t="s">
         <v>66</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1895,7 +1318,7 @@
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1904,7 +1327,7 @@
       <c r="D3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="3" t="s">
         <v>66</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1916,51 +1339,49 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.amazon.in/"/>
-    <hyperlink ref="D2" r:id="rId2" display="Damco@124"/>
-    <hyperlink ref="E2" r:id="rId3" display="XYZTestr@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.amazon.in/"/>
-    <hyperlink ref="D3" r:id="rId2" display="Damco@123"/>
-    <hyperlink ref="E3" r:id="rId3" display="XYZTestr@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="D3" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="E3" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="G2 F10 C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.859375" customWidth="1"/>
-    <col min="2" max="3" width="15.2890625" customWidth="1"/>
-    <col min="4" max="4" width="27.421875" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="1025" width="8.671875" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" customWidth="1"/>
+    <col min="6" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="8" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1999,24 +1420,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="G2 F10 C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1025" width="8.671875" customWidth="1"/>
+    <col min="1" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2025,33 +1444,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="G2 F10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="38.703125" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" customWidth="1"/>
+    <col min="2" max="2" width="38.7265625" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="9.421875" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.8671875" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="1025" width="8.671875" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="8" max="8" width="16.90625" customWidth="1"/>
+    <col min="9" max="9" width="16.1796875" customWidth="1"/>
+    <col min="10" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2072,10 +1489,10 @@
       <c r="A2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -2086,10 +1503,10 @@
       <c r="A3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -2098,41 +1515,47 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://release.getcheddarup.com/login/"/>
-    <hyperlink ref="C2" r:id="rId2" display="sarahsmith@example.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="tester1"/>
-    <hyperlink ref="B3" r:id="rId1" display="https://release.getcheddarup.com/login/"/>
-    <hyperlink ref="C3" r:id="rId2" display="sarahsmith@example.com"/>
-    <hyperlink ref="D3" r:id="rId3" display="tester123"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="D3" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.3125" customWidth="1"/>
-    <col min="3" max="6" width="21.8203125" customWidth="1"/>
-    <col min="7" max="7" width="11.9375" customWidth="1"/>
-    <col min="8" max="8" width="18.46875" customWidth="1"/>
-    <col min="9" max="13" width="20.828125" customWidth="1"/>
-    <col min="14" max="17" width="11.5234375" hidden="1"/>
-    <col min="18" max="1028" width="8.671875" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
+    <col min="3" max="3" width="51.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.81640625" customWidth="1"/>
+    <col min="7" max="7" width="11.90625" customWidth="1"/>
+    <col min="8" max="8" width="18.453125" customWidth="1"/>
+    <col min="9" max="12" width="20.81640625" customWidth="1"/>
+    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.54296875" hidden="1"/>
+    <col min="15" max="15" width="9" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.1796875" customWidth="1"/>
+    <col min="18" max="18" width="13" customWidth="1"/>
+    <col min="19" max="19" width="12.6328125" customWidth="1"/>
+    <col min="20" max="1028" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2151,98 +1574,140 @@
       <c r="F1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="2" t="s">
+      <c r="N1" s="6"/>
+      <c r="O1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="6"/>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="14">
         <v>9717254315</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="17">
         <v>2345</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="P3" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" display="demo@yahooo.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="https://testingxperts-5d-dev-ed.develop.my.salesforce.com"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="C3" r:id="rId3" display="https://testingxperts61-dev-ed.develop.my.salesforce.com/" xr:uid="{87C2E6C4-6075-4B2F-80CC-D6518A75629B}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{173185E0-5DD7-4354-AF5C-FF452329EF6E}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Creating Leads and converting
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SalesForceAutomation\SalesforceAutomation\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CD26B5-CE07-4799-B135-D2CCE074E315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6830" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WebTestData" sheetId="1" r:id="rId1"/>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="115">
   <si>
     <t>TestData</t>
   </si>
@@ -314,15 +320,6 @@
     <t>Stage</t>
   </si>
   <si>
-    <t>CamapaignName</t>
-  </si>
-  <si>
-    <t>EditCampaignName</t>
-  </si>
-  <si>
-    <t>ParentCampaign</t>
-  </si>
-  <si>
     <t>QuoteType</t>
   </si>
   <si>
@@ -353,32 +350,35 @@
     <t>Prospecting</t>
   </si>
   <si>
-    <t>YearABc</t>
-  </si>
-  <si>
-    <t>Year1</t>
-  </si>
-  <si>
-    <t>Festival</t>
-  </si>
-  <si>
     <t>Quote</t>
   </si>
   <si>
     <t>demo@yahooo.com</t>
+  </si>
+  <si>
+    <t>CityName</t>
+  </si>
+  <si>
+    <t>Anil</t>
+  </si>
+  <si>
+    <t>anil53756@gmail.com</t>
+  </si>
+  <si>
+    <t>https://testingxperts61-dev-ed.develop.my.salesforce.com</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Sharma@123#&amp;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -412,155 +412,13 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -581,210 +439,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FF8EB4E3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF8EB4E3"/>
         <bgColor rgb="FF95B3D7"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -824,30 +484,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -859,312 +495,68 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color auto="1"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color auto="1"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color auto="1"/>
       </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1237,6 +629,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1494,42 +889,42 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="G2 F10 A1"/>
+      <selection sqref="G2 F10 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.8636363636364" customWidth="1"/>
-    <col min="2" max="3" width="15.2909090909091" customWidth="1"/>
-    <col min="4" max="4" width="27.4181818181818" customWidth="1"/>
-    <col min="5" max="5" width="9.41818181818182" customWidth="1"/>
-    <col min="6" max="6" width="10.8545454545455" customWidth="1"/>
-    <col min="7" max="7" width="28.1363636363636" customWidth="1"/>
-    <col min="8" max="8" width="26.2909090909091" customWidth="1"/>
-    <col min="9" max="9" width="10.1363636363636" customWidth="1"/>
-    <col min="10" max="10" width="9.70909090909091" customWidth="1"/>
-    <col min="11" max="13" width="8.67272727272727" customWidth="1"/>
-    <col min="14" max="14" width="12.7090909090909" customWidth="1"/>
-    <col min="15" max="15" width="21.1363636363636" customWidth="1"/>
-    <col min="16" max="16" width="8.67272727272727" customWidth="1"/>
-    <col min="17" max="17" width="12.2909090909091" customWidth="1"/>
-    <col min="18" max="18" width="26.2909090909091" customWidth="1"/>
-    <col min="19" max="19" width="19.7090909090909" customWidth="1"/>
-    <col min="20" max="20" width="15.5727272727273" customWidth="1"/>
-    <col min="21" max="21" width="14.8636363636364" customWidth="1"/>
-    <col min="22" max="22" width="18.7090909090909" customWidth="1"/>
-    <col min="23" max="23" width="21.1363636363636" customWidth="1"/>
-    <col min="24" max="24" width="32.2909090909091" customWidth="1"/>
-    <col min="25" max="1025" width="8.67272727272727" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" customWidth="1"/>
+    <col min="7" max="7" width="28.1796875" customWidth="1"/>
+    <col min="8" max="8" width="26.26953125" customWidth="1"/>
+    <col min="9" max="9" width="10.08984375" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" customWidth="1"/>
+    <col min="11" max="13" width="8.6328125" customWidth="1"/>
+    <col min="14" max="14" width="12.7265625" customWidth="1"/>
+    <col min="15" max="15" width="21.1796875" customWidth="1"/>
+    <col min="16" max="16" width="8.6328125" customWidth="1"/>
+    <col min="17" max="17" width="12.26953125" customWidth="1"/>
+    <col min="18" max="18" width="26.26953125" customWidth="1"/>
+    <col min="19" max="19" width="19.7265625" customWidth="1"/>
+    <col min="20" max="20" width="15.54296875" customWidth="1"/>
+    <col min="21" max="21" width="14.81640625" customWidth="1"/>
+    <col min="22" max="22" width="18.7265625" customWidth="1"/>
+    <col min="23" max="23" width="21.1796875" customWidth="1"/>
+    <col min="24" max="24" width="32.26953125" customWidth="1"/>
+    <col min="25" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -1607,168 +1002,166 @@
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4" t="s">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="T3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="U3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="V3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="W3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="X3" s="2" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="G2 F10 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.70909090909091" customWidth="1"/>
-    <col min="2" max="2" width="12.4181818181818" customWidth="1"/>
-    <col min="3" max="3" width="32.2909090909091" customWidth="1"/>
-    <col min="4" max="4" width="12.5727272727273" customWidth="1"/>
-    <col min="5" max="7" width="8.67272727272727" customWidth="1"/>
-    <col min="8" max="8" width="17.7090909090909" customWidth="1"/>
-    <col min="9" max="1025" width="8.67272727272727" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="32.26953125" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1"/>
+    <col min="5" max="7" width="8.6328125" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" customWidth="1"/>
+    <col min="9" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1797,84 +1190,82 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" ht="15.5" spans="1:8">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:8" ht="15.5">
+      <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="9">
         <v>9888882626</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" ht="15.5" spans="1:8">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:8" ht="15.5">
+      <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="9">
         <v>9888882626</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="10" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="w@maxbupa.com"/>
-    <hyperlink ref="H3" r:id="rId1" display="w@maxbupa.com"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="G2 F10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.2909090909091" customWidth="1"/>
-    <col min="2" max="2" width="27.5818181818182" customWidth="1"/>
-    <col min="3" max="3" width="12.4181818181818" customWidth="1"/>
-    <col min="4" max="4" width="12.7090909090909" customWidth="1"/>
-    <col min="5" max="5" width="29.7090909090909" customWidth="1"/>
-    <col min="6" max="6" width="8.67272727272727" customWidth="1"/>
-    <col min="7" max="7" width="45.5727272727273" customWidth="1"/>
-    <col min="8" max="1025" width="8.67272727272727" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" customWidth="1"/>
+    <col min="2" max="2" width="27.54296875" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" customWidth="1"/>
+    <col min="5" max="5" width="29.7265625" customWidth="1"/>
+    <col min="6" max="6" width="8.6328125" customWidth="1"/>
+    <col min="7" max="7" width="45.54296875" customWidth="1"/>
+    <col min="8" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1901,145 +1292,141 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.amazon.in/"/>
-    <hyperlink ref="D2" r:id="rId2" display="Damco@124"/>
-    <hyperlink ref="E2" r:id="rId3" display="XYZTestr@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.amazon.in/"/>
-    <hyperlink ref="D3" r:id="rId2" display="Damco@123"/>
-    <hyperlink ref="E3" r:id="rId3" display="XYZTestr@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="D3" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="E3" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="G2 F10 C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.8636363636364" customWidth="1"/>
-    <col min="2" max="3" width="15.2909090909091" customWidth="1"/>
-    <col min="4" max="4" width="27.4181818181818" customWidth="1"/>
-    <col min="5" max="5" width="16.5727272727273" customWidth="1"/>
-    <col min="6" max="1025" width="8.67272727272727" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" customWidth="1"/>
+    <col min="6" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2048,7 +1435,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1025" width="8.67272727272727" customWidth="1"/>
+    <col min="1" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2057,33 +1444,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="G2 F10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.70909090909091" customWidth="1"/>
-    <col min="2" max="2" width="38.7" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" customWidth="1"/>
+    <col min="2" max="2" width="38.7265625" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="9.41818181818182" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="16.7090909090909" customWidth="1"/>
-    <col min="8" max="8" width="16.8636363636364" customWidth="1"/>
-    <col min="9" max="9" width="16.1363636363636" customWidth="1"/>
-    <col min="10" max="1025" width="8.67272727272727" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="8" max="8" width="16.90625" customWidth="1"/>
+    <col min="9" max="9" width="16.1796875" customWidth="1"/>
+    <col min="10" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2101,73 +1486,76 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://release.getcheddarup.com/login/"/>
-    <hyperlink ref="C2" r:id="rId2" display="sarahsmith@example.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="tester1"/>
-    <hyperlink ref="B3" r:id="rId1" display="https://release.getcheddarup.com/login/"/>
-    <hyperlink ref="C3" r:id="rId2" display="sarahsmith@example.com"/>
-    <hyperlink ref="D3" r:id="rId3" display="tester123"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="D3" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:V2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.5727272727273" customWidth="1"/>
-    <col min="2" max="2" width="19.3090909090909" customWidth="1"/>
-    <col min="3" max="6" width="21.8181818181818" customWidth="1"/>
-    <col min="7" max="7" width="11.9363636363636" customWidth="1"/>
-    <col min="8" max="8" width="18.4727272727273" customWidth="1"/>
-    <col min="9" max="16" width="20.8272727272727" customWidth="1"/>
-    <col min="17" max="19" width="11.5272727272727" customWidth="1"/>
-    <col min="20" max="20" width="2.81818181818182" customWidth="1"/>
-    <col min="21" max="21" width="18.1818181818182" customWidth="1"/>
-    <col min="22" max="22" width="17.8181818181818" customWidth="1"/>
-    <col min="23" max="1031" width="8.67272727272727" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
+    <col min="3" max="3" width="51.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.81640625" customWidth="1"/>
+    <col min="7" max="7" width="11.90625" customWidth="1"/>
+    <col min="8" max="8" width="18.453125" customWidth="1"/>
+    <col min="9" max="12" width="20.81640625" customWidth="1"/>
+    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.54296875" hidden="1"/>
+    <col min="15" max="15" width="9" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.1796875" customWidth="1"/>
+    <col min="18" max="18" width="13" customWidth="1"/>
+    <col min="19" max="19" width="12.6328125" customWidth="1"/>
+    <col min="20" max="1028" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2186,111 +1574,132 @@
       <c r="F1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="6"/>
+      <c r="O1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="6"/>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="B2" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="C2" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-    </row>
-    <row r="2" spans="1:22">
-      <c r="A2" s="4" t="s">
+      <c r="D2" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="E2" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="F2" s="14">
+        <v>9717254315</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="H2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="J2" s="17">
+        <v>2345</v>
+      </c>
+      <c r="K2" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="7">
-        <v>9717254315</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="L2" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="9" t="s">
+      <c r="M2" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="J2" s="11">
-        <v>2345</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="L2" s="12" t="s">
+      <c r="N2" s="18"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="M2" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="O2" s="9" t="s">
+      <c r="P3" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="P2" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" display="demo@yahooo.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="https://testingxperts-5d-dev-ed.develop.my.salesforce.com"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="C3" r:id="rId3" display="https://testingxperts61-dev-ed.develop.my.salesforce.com/" xr:uid="{87C2E6C4-6075-4B2F-80CC-D6518A75629B}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{173185E0-5DD7-4354-AF5C-FF452329EF6E}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2300,6 +1709,5 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Committing files for Forecasting Module - Create Users for forecasting
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitu Yadav\OneDrive\Documents\Selenium Project\SalesforceAutomation\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41717990-E327-4636-BB98-796534E65784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11440" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WebTestData" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="124">
   <si>
     <t>TestData</t>
   </si>
@@ -349,19 +354,58 @@
   </si>
   <si>
     <t>demo@yahooo.com</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>Nickname</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Nisha</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>nsharma</t>
+  </si>
+  <si>
+    <t>ynitu913@gmail.com</t>
+  </si>
+  <si>
+    <t>NiaSharma</t>
+  </si>
+  <si>
+    <t>Nia</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>n_username</t>
+  </si>
+  <si>
+    <t>https://testingxperts-5d-dev-ed.develop.my.salesforce.com/</t>
+  </si>
+  <si>
+    <t>Forecast_URL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -395,155 +439,25 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -570,192 +484,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -809,330 +543,52 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="24">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-  </cellStyleXfs>
-  <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="48" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1205,6 +661,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1462,42 +921,42 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="G2 F10 A1"/>
+      <selection sqref="G2 F10 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.859375" customWidth="1"/>
-    <col min="2" max="3" width="15.2890625" customWidth="1"/>
-    <col min="4" max="4" width="27.421875" customWidth="1"/>
-    <col min="5" max="5" width="9.421875" customWidth="1"/>
-    <col min="6" max="6" width="10.8515625" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="28.140625" customWidth="1"/>
-    <col min="8" max="8" width="26.2890625" customWidth="1"/>
-    <col min="9" max="9" width="10.1328125" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="13" width="8.671875" customWidth="1"/>
+    <col min="11" max="13" width="8.7109375" customWidth="1"/>
     <col min="14" max="14" width="12.7109375" customWidth="1"/>
     <col min="15" max="15" width="21.140625" customWidth="1"/>
-    <col min="16" max="16" width="8.671875" customWidth="1"/>
-    <col min="17" max="17" width="12.2890625" customWidth="1"/>
-    <col min="18" max="18" width="26.2890625" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" customWidth="1"/>
+    <col min="18" max="18" width="26.28515625" customWidth="1"/>
     <col min="19" max="19" width="19.7109375" customWidth="1"/>
     <col min="20" max="20" width="15.5703125" customWidth="1"/>
-    <col min="21" max="21" width="14.859375" customWidth="1"/>
+    <col min="21" max="21" width="14.85546875" customWidth="1"/>
     <col min="22" max="22" width="18.7109375" customWidth="1"/>
     <col min="23" max="23" width="21.140625" customWidth="1"/>
-    <col min="24" max="24" width="32.2890625" customWidth="1"/>
-    <col min="25" max="1025" width="8.671875" customWidth="1"/>
+    <col min="24" max="24" width="32.28515625" customWidth="1"/>
+    <col min="25" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -1587,7 +1046,7 @@
       <c r="D2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1661,7 +1120,7 @@
       <c r="D3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1713,30 +1172,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="G2 F10 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.421875" customWidth="1"/>
-    <col min="3" max="3" width="32.2890625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="7" width="8.671875" customWidth="1"/>
+    <col min="5" max="7" width="8.7109375" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="1025" width="8.671875" customWidth="1"/>
+    <col min="9" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1765,84 +1222,82 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" ht="14.8" spans="1:8">
+    <row r="2" spans="1:8" ht="15.75">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="14">
         <v>9888882626</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="15" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" ht="14.8" spans="1:8">
+    <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="14">
         <v>9888882626</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="15" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="w@maxbupa.com"/>
-    <hyperlink ref="H3" r:id="rId1" display="w@maxbupa.com"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="G2 F10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.2890625" customWidth="1"/>
-    <col min="2" max="2" width="27.578125" customWidth="1"/>
-    <col min="3" max="3" width="12.421875" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.671875" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
     <col min="7" max="7" width="45.5703125" customWidth="1"/>
-    <col min="8" max="1025" width="8.671875" customWidth="1"/>
+    <col min="8" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1872,7 +1327,7 @@
       <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1881,7 +1336,7 @@
       <c r="D2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="4" t="s">
         <v>66</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1895,7 +1350,7 @@
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1904,7 +1359,7 @@
       <c r="D3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="4" t="s">
         <v>66</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1916,51 +1371,49 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.amazon.in/"/>
-    <hyperlink ref="D2" r:id="rId2" display="Damco@124"/>
-    <hyperlink ref="E2" r:id="rId3" display="XYZTestr@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.amazon.in/"/>
-    <hyperlink ref="D3" r:id="rId2" display="Damco@123"/>
-    <hyperlink ref="E3" r:id="rId3" display="XYZTestr@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="D3" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="E3" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="G2 F10 C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.859375" customWidth="1"/>
-    <col min="2" max="3" width="15.2890625" customWidth="1"/>
-    <col min="4" max="4" width="27.421875" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="1025" width="8.671875" customWidth="1"/>
+    <col min="6" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1999,24 +1452,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="G2 F10 C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.671875" customWidth="1"/>
+    <col min="1" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2025,33 +1476,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="G2 F10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="38.703125" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="9.421875" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.8671875" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
     <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="1025" width="8.671875" customWidth="1"/>
+    <col min="10" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2072,10 +1521,10 @@
       <c r="A2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="4" t="s">
         <v>86</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -2086,10 +1535,10 @@
       <c r="A3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="4" t="s">
         <v>86</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -2098,41 +1547,49 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://release.getcheddarup.com/login/"/>
-    <hyperlink ref="C2" r:id="rId2" display="sarahsmith@example.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="tester1"/>
-    <hyperlink ref="B3" r:id="rId1" display="https://release.getcheddarup.com/login/"/>
-    <hyperlink ref="C3" r:id="rId2" display="sarahsmith@example.com"/>
-    <hyperlink ref="D3" r:id="rId3" display="tester123"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="D3" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.3125" customWidth="1"/>
-    <col min="3" max="6" width="21.8203125" customWidth="1"/>
-    <col min="7" max="7" width="11.9375" customWidth="1"/>
-    <col min="8" max="8" width="18.46875" customWidth="1"/>
-    <col min="9" max="13" width="20.828125" customWidth="1"/>
-    <col min="14" max="17" width="11.5234375" hidden="1"/>
-    <col min="18" max="1028" width="8.671875" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="4" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="12" width="20.85546875" customWidth="1"/>
+    <col min="13" max="13" width="25.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" customWidth="1"/>
+    <col min="20" max="20" width="16.140625" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" customWidth="1"/>
+    <col min="22" max="22" width="59.5703125" customWidth="1"/>
+    <col min="23" max="1028" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2172,19 +1629,47 @@
       <c r="M1" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
+      <c r="N1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q1" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="T1" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="U1" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="V1" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="W1" s="20"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>101</v>
+      <c r="C2" s="17" t="s">
+        <v>122</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>102</v>
@@ -2213,36 +1698,60 @@
       <c r="L2" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
+      <c r="N2" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q2" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="R2" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="W2" s="20"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" display="demo@yahooo.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="https://testingxperts-5d-dev-ed.develop.my.salesforce.com"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{19EF7A34-BF39-4139-9B7E-89FEB8E70FCA}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commiting the select parent , add leads workflow
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6830" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView windowWidth="19200" windowHeight="6830" tabRatio="500" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="WebTestData" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="117">
   <si>
     <t>TestData</t>
   </si>
@@ -323,6 +323,9 @@
     <t>ParentCampaign</t>
   </si>
   <si>
+    <t>LeadName</t>
+  </si>
+  <si>
     <t>QuoteType</t>
   </si>
   <si>
@@ -353,13 +356,16 @@
     <t>Prospecting</t>
   </si>
   <si>
-    <t>YearABc</t>
+    <t>YearABC</t>
   </si>
   <si>
     <t>Year1</t>
   </si>
   <si>
     <t>Festival</t>
+  </si>
+  <si>
+    <t>Anil</t>
   </si>
   <si>
     <t>Quote</t>
@@ -1091,7 +1097,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1099,14 +1105,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1619,7 +1626,7 @@
       <c r="D2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="17" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -1693,7 +1700,7 @@
       <c r="D3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="17" t="s">
         <v>27</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -1801,25 +1808,25 @@
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="20">
         <v>9888882626</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="21" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1827,21 +1834,21 @@
       <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="20">
         <v>9888882626</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="21" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1904,7 +1911,7 @@
       <c r="A2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>63</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1913,7 +1920,7 @@
       <c r="D2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="17" t="s">
         <v>66</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -1927,7 +1934,7 @@
       <c r="A3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>63</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1936,7 +1943,7 @@
       <c r="D3" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="17" t="s">
         <v>66</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -1980,19 +1987,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="19" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2104,10 +2111,10 @@
       <c r="A2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>86</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -2118,10 +2125,10 @@
       <c r="A3" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="17" t="s">
         <v>86</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -2146,10 +2153,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
@@ -2159,15 +2166,15 @@
     <col min="3" max="6" width="21.8181818181818" customWidth="1"/>
     <col min="7" max="7" width="11.9363636363636" customWidth="1"/>
     <col min="8" max="8" width="18.4727272727273" customWidth="1"/>
-    <col min="9" max="16" width="20.8272727272727" customWidth="1"/>
-    <col min="17" max="19" width="11.5272727272727" customWidth="1"/>
-    <col min="20" max="20" width="2.81818181818182" customWidth="1"/>
-    <col min="21" max="21" width="18.1818181818182" customWidth="1"/>
-    <col min="22" max="22" width="17.8181818181818" customWidth="1"/>
-    <col min="23" max="1031" width="8.67272727272727" customWidth="1"/>
+    <col min="9" max="17" width="20.8272727272727" customWidth="1"/>
+    <col min="18" max="20" width="11.5272727272727" customWidth="1"/>
+    <col min="21" max="21" width="2.81818181818182" customWidth="1"/>
+    <col min="22" max="22" width="18.1818181818182" customWidth="1"/>
+    <col min="23" max="23" width="17.8181818181818" customWidth="1"/>
+    <col min="24" max="1032" width="8.67272727272727" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2201,10 +2208,10 @@
       <c r="K1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="11" t="s">
         <v>98</v>
       </c>
       <c r="N1" s="3" t="s">
@@ -2213,74 +2220,82 @@
       <c r="O1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="U1" s="14"/>
+      <c r="Q1" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
       <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:23">
       <c r="A2" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="7">
+        <v>107</v>
+      </c>
+      <c r="F2" s="8">
         <v>9717254315</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="J2" s="11">
+      <c r="I2" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="12">
         <v>2345</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="L2" s="12" t="s">
+      <c r="K2" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="L2" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="M2" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="N2" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="O2" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
+      <c r="P2" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" display="demo@yahooo.com"/>
+    <hyperlink ref="Q2" r:id="rId1" display="demo@yahooo.com"/>
     <hyperlink ref="C2" r:id="rId2" display="https://testingxperts-5d-dev-ed.develop.my.salesforce.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="xperttesting3@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId4" display="Tiger@2024"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -2293,7 +2308,7 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updating the test data sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6830" tabRatio="500" firstSheet="3" activeTab="7"/>
+    <workbookView windowWidth="19200" windowHeight="6830" tabRatio="500" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="WebTestData" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="122">
   <si>
     <t>TestData</t>
   </si>
@@ -332,6 +332,9 @@
     <t>ContactEmail</t>
   </si>
   <si>
+    <t>CityName</t>
+  </si>
+  <si>
     <t>TestData1</t>
   </si>
   <si>
@@ -372,6 +375,18 @@
   </si>
   <si>
     <t>demo@yahooo.com</t>
+  </si>
+  <si>
+    <t>https://testingxperts61-dev-ed.develop.my.salesforce.com</t>
+  </si>
+  <si>
+    <t>anil53756@gmail.com</t>
+  </si>
+  <si>
+    <t>Sharma@123#&amp;</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
   </si>
 </sst>
 </file>
@@ -384,7 +399,7 @@
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -404,6 +419,12 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
@@ -964,19 +985,16 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -985,119 +1003,122 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1109,17 +1130,22 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1626,7 +1652,7 @@
       <c r="D2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="22" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -1700,7 +1726,7 @@
       <c r="D3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="22" t="s">
         <v>27</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -1808,25 +1834,25 @@
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="25">
         <v>9888882626</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="26" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1834,21 +1860,21 @@
       <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="25">
         <v>9888882626</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20" t="s">
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="26" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1911,7 +1937,7 @@
       <c r="A2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="22" t="s">
         <v>63</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1920,7 +1946,7 @@
       <c r="D2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="22" t="s">
         <v>66</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -1934,7 +1960,7 @@
       <c r="A3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="22" t="s">
         <v>63</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1943,7 +1969,7 @@
       <c r="D3" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="22" t="s">
         <v>66</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -1987,19 +2013,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="24" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2111,10 +2137,10 @@
       <c r="A2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="22" t="s">
         <v>86</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -2125,10 +2151,10 @@
       <c r="A3" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="22" t="s">
         <v>86</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -2153,13 +2179,13 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="20.5727272727273" customWidth="1"/>
     <col min="2" max="2" width="19.3090909090909" customWidth="1"/>
@@ -2208,10 +2234,10 @@
       <c r="K1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="13" t="s">
         <v>98</v>
       </c>
       <c r="N1" s="3" t="s">
@@ -2223,72 +2249,110 @@
       <c r="P1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
+      <c r="R1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="T1" s="13"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F2" s="8">
         <v>9717254315</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="J2" s="12">
+        <v>110</v>
+      </c>
+      <c r="J2" s="14">
         <v>2345</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="L2" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="L2" s="11" t="s">
         <v>112</v>
       </c>
+      <c r="M2" s="11" t="s">
+        <v>113</v>
+      </c>
       <c r="N2" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="P2" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q2" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="19"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="Q2" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
+      <c r="S3" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="T3" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2296,6 +2360,8 @@
     <hyperlink ref="C2" r:id="rId2" display="https://testingxperts-5d-dev-ed.develop.my.salesforce.com"/>
     <hyperlink ref="D2" r:id="rId3" display="xperttesting3@gmail.com"/>
     <hyperlink ref="E2" r:id="rId4" display="Tiger@2024"/>
+    <hyperlink ref="C3" r:id="rId5" display="https://testingxperts61-dev-ed.develop.my.salesforce.com"/>
+    <hyperlink ref="E3" r:id="rId6" display="Sharma@123#&amp;"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -2308,7 +2374,7 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Committing the code for the cases and create, edit leads and search lead
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="125">
   <si>
     <t>TestData</t>
   </si>
@@ -368,6 +368,12 @@
     <t>demo@yahooo.com</t>
   </si>
   <si>
+    <t>Anil</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
     <t>YearABC</t>
   </si>
   <si>
@@ -375,9 +381,6 @@
   </si>
   <si>
     <t>Year1</t>
-  </si>
-  <si>
-    <t>Anil</t>
   </si>
   <si>
     <t>Name</t>
@@ -2182,8 +2185,8 @@
   <sheetPr/>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -2312,22 +2315,26 @@
         <v>114</v>
       </c>
       <c r="N2" s="14"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
+      <c r="O2" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>116</v>
+      </c>
       <c r="Q2" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="T2" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="R2" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>118</v>
-      </c>
       <c r="U2" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -2336,13 +2343,13 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
@@ -2354,16 +2361,18 @@
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
       <c r="O3" s="16" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="Q3" s="16"/>
       <c r="R3" s="16"/>
       <c r="S3" s="16"/>
       <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
+      <c r="U3" s="10" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="10" spans="21:21">
       <c r="U10" s="10"/>

</xml_diff>

<commit_message>
Added service support files_19/04_added
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -1091,10 +1091,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1607,140 +1606,140 @@
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4" t="s">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="T3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="U3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="V3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="W3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="X3" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1798,50 +1797,50 @@
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="18">
         <v>9888882626</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="19" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" ht="15.5" spans="1:8">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="18">
         <v>9888882626</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="19" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1901,48 +1900,48 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1980,53 +1979,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2101,30 +2100,30 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2146,10 +2145,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
@@ -2160,14 +2159,12 @@
     <col min="7" max="7" width="11.9363636363636" customWidth="1"/>
     <col min="8" max="8" width="18.4727272727273" customWidth="1"/>
     <col min="9" max="16" width="20.8272727272727" customWidth="1"/>
-    <col min="17" max="19" width="11.5272727272727" customWidth="1"/>
-    <col min="20" max="20" width="2.81818181818182" customWidth="1"/>
-    <col min="21" max="21" width="18.1818181818182" customWidth="1"/>
-    <col min="22" max="22" width="17.8181818181818" customWidth="1"/>
-    <col min="23" max="1031" width="8.67272727272727" customWidth="1"/>
+    <col min="17" max="17" width="18.1818181818182" customWidth="1"/>
+    <col min="18" max="18" width="17.8181818181818" customWidth="1"/>
+    <col min="19" max="1027" width="8.67272727272727" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2189,93 +2186,87 @@
       <c r="G1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
     </row>
-    <row r="2" spans="1:22">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:18">
+      <c r="A2" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>9717254315</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="10">
         <v>2345</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="P2" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added all files 19/04 for service support
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="118">
   <si>
     <t>TestData</t>
   </si>
@@ -329,6 +329,12 @@
     <t>ContactEmail</t>
   </si>
   <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
     <t>TestData1</t>
   </si>
   <si>
@@ -366,6 +372,9 @@
   </si>
   <si>
     <t>demo@yahooo.com</t>
+  </si>
+  <si>
+    <t>New</t>
   </si>
 </sst>
 </file>
@@ -560,7 +569,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -577,18 +586,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF95B3D7"/>
         <bgColor rgb="FF8EB4E3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FF8EB4E3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -967,7 +964,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -991,16 +988,16 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1009,89 +1006,89 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1105,11 +1102,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
@@ -1618,7 +1613,7 @@
       <c r="D2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="13" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1692,7 +1687,7 @@
       <c r="D3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="13" t="s">
         <v>27</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1800,25 +1795,25 @@
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="16">
         <v>9888882626</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="17" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1826,21 +1821,21 @@
       <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="16">
         <v>9888882626</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="17" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1903,7 +1898,7 @@
       <c r="A2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>63</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1912,7 +1907,7 @@
       <c r="D2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="13" t="s">
         <v>66</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1926,7 +1921,7 @@
       <c r="A3" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="13" t="s">
         <v>63</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1935,7 +1930,7 @@
       <c r="D3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="13" t="s">
         <v>66</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1979,19 +1974,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2103,10 +2098,10 @@
       <c r="A2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>86</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -2117,10 +2112,10 @@
       <c r="A3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="13" t="s">
         <v>86</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -2147,8 +2142,8 @@
   <sheetPr/>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
@@ -2213,60 +2208,68 @@
       <c r="P1" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
+      <c r="Q1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F2" s="6">
         <v>9717254315</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="J2" s="10">
         <v>2345</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+        <v>116</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added all files 24/04 for service support
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6830" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView windowWidth="19200" windowHeight="6800" tabRatio="500" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="WebTestData" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,25 @@
     <sheet name="Salesforce" sheetId="7" r:id="rId7"/>
     <sheet name="SalesforceLogin" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="140">
   <si>
     <t>TestData</t>
   </si>
@@ -314,19 +327,43 @@
     <t>Stage</t>
   </si>
   <si>
-    <t>CamapaignName</t>
+    <t>QuoteType</t>
+  </si>
+  <si>
+    <t>ContactEmail</t>
+  </si>
+  <si>
+    <t>CityName</t>
+  </si>
+  <si>
+    <t>CampaignName</t>
+  </si>
+  <si>
+    <t>ParentCampaign</t>
   </si>
   <si>
     <t>EditCampaignName</t>
   </si>
   <si>
-    <t>ParentCampaign</t>
-  </si>
-  <si>
-    <t>QuoteType</t>
-  </si>
-  <si>
-    <t>ContactEmail</t>
+    <t>LeadName</t>
+  </si>
+  <si>
+    <t>FieldValue</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>n_username</t>
+  </si>
+  <si>
+    <t>Nickname</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>Department</t>
   </si>
   <si>
     <t>status</t>
@@ -359,35 +396,77 @@
     <t>Prospecting</t>
   </si>
   <si>
-    <t>YearABc</t>
+    <t>Quote</t>
+  </si>
+  <si>
+    <t>demo@yahooo.com</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>YearABC</t>
+  </si>
+  <si>
+    <t>Festival</t>
   </si>
   <si>
     <t>Year1</t>
   </si>
   <si>
-    <t>Festival</t>
-  </si>
-  <si>
-    <t>Quote</t>
-  </si>
-  <si>
-    <t>demo@yahooo.com</t>
+    <t>Anil</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Nisha</t>
+  </si>
+  <si>
+    <t>nsharma</t>
+  </si>
+  <si>
+    <t>ynitu913@gmail.com</t>
+  </si>
+  <si>
+    <t>NiaSharma</t>
+  </si>
+  <si>
+    <t>Nia</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>Sales</t>
   </si>
   <si>
     <t>New</t>
+  </si>
+  <si>
+    <t>https://testingxperts61-dev-ed.develop.my.salesforce.com</t>
+  </si>
+  <si>
+    <t>anil53756@gmail.com</t>
+  </si>
+  <si>
+    <t>Sharma@123#&amp;</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -409,6 +488,30 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -421,9 +524,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -435,13 +540,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -590,6 +688,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF8EB4E3"/>
         <bgColor rgb="FF95B3D7"/>
       </patternFill>
@@ -656,12 +760,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -781,7 +879,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -821,11 +919,33 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -836,21 +956,6 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -955,158 +1060,180 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="6" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="6" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1502,28 +1629,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="14.8636363636364" customWidth="1"/>
-    <col min="2" max="3" width="15.2909090909091" customWidth="1"/>
-    <col min="4" max="4" width="27.4181818181818" customWidth="1"/>
-    <col min="5" max="5" width="9.41818181818182" customWidth="1"/>
-    <col min="6" max="6" width="10.8545454545455" customWidth="1"/>
-    <col min="7" max="7" width="28.1363636363636" customWidth="1"/>
-    <col min="8" max="8" width="26.2909090909091" customWidth="1"/>
-    <col min="9" max="9" width="10.1363636363636" customWidth="1"/>
-    <col min="10" max="10" width="9.70909090909091" customWidth="1"/>
-    <col min="11" max="13" width="8.67272727272727" customWidth="1"/>
-    <col min="14" max="14" width="12.7090909090909" customWidth="1"/>
-    <col min="15" max="15" width="21.1363636363636" customWidth="1"/>
-    <col min="16" max="16" width="8.67272727272727" customWidth="1"/>
-    <col min="17" max="17" width="12.2909090909091" customWidth="1"/>
-    <col min="18" max="18" width="26.2909090909091" customWidth="1"/>
-    <col min="19" max="19" width="19.7090909090909" customWidth="1"/>
-    <col min="20" max="20" width="15.5727272727273" customWidth="1"/>
-    <col min="21" max="21" width="14.8636363636364" customWidth="1"/>
-    <col min="22" max="22" width="18.7090909090909" customWidth="1"/>
-    <col min="23" max="23" width="21.1363636363636" customWidth="1"/>
-    <col min="24" max="24" width="32.2909090909091" customWidth="1"/>
-    <col min="25" max="1025" width="8.67272727272727" customWidth="1"/>
+    <col min="1" max="1" width="14.8181818181818" customWidth="1"/>
+    <col min="2" max="3" width="15.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="27.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="9.45454545454546" customWidth="1"/>
+    <col min="6" max="6" width="10.8181818181818" customWidth="1"/>
+    <col min="7" max="7" width="28.1818181818182" customWidth="1"/>
+    <col min="8" max="8" width="26.2727272727273" customWidth="1"/>
+    <col min="9" max="9" width="10.0909090909091" customWidth="1"/>
+    <col min="10" max="10" width="9.72727272727273" customWidth="1"/>
+    <col min="11" max="13" width="8.63636363636364" customWidth="1"/>
+    <col min="14" max="14" width="12.7272727272727" customWidth="1"/>
+    <col min="15" max="15" width="21.1818181818182" customWidth="1"/>
+    <col min="16" max="16" width="8.63636363636364" customWidth="1"/>
+    <col min="17" max="17" width="12.2727272727273" customWidth="1"/>
+    <col min="18" max="18" width="26.2727272727273" customWidth="1"/>
+    <col min="19" max="19" width="19.7272727272727" customWidth="1"/>
+    <col min="20" max="20" width="15.5454545454545" customWidth="1"/>
+    <col min="21" max="21" width="14.8181818181818" customWidth="1"/>
+    <col min="22" max="22" width="18.7272727272727" customWidth="1"/>
+    <col min="23" max="23" width="21.1818181818182" customWidth="1"/>
+    <col min="24" max="24" width="32.2727272727273" customWidth="1"/>
+    <col min="25" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -1601,140 +1728,140 @@
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3" t="s">
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="U3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="V3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="W3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="X3" s="10" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1756,13 +1883,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="9.70909090909091" customWidth="1"/>
-    <col min="2" max="2" width="12.4181818181818" customWidth="1"/>
-    <col min="3" max="3" width="32.2909090909091" customWidth="1"/>
-    <col min="4" max="4" width="12.5727272727273" customWidth="1"/>
-    <col min="5" max="7" width="8.67272727272727" customWidth="1"/>
-    <col min="8" max="8" width="17.7090909090909" customWidth="1"/>
-    <col min="9" max="1025" width="8.67272727272727" customWidth="1"/>
+    <col min="1" max="1" width="9.72727272727273" customWidth="1"/>
+    <col min="2" max="2" width="12.4545454545455" customWidth="1"/>
+    <col min="3" max="3" width="32.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="12.5454545454545" customWidth="1"/>
+    <col min="5" max="7" width="8.63636363636364" customWidth="1"/>
+    <col min="8" max="8" width="17.7272727272727" customWidth="1"/>
+    <col min="9" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1792,50 +1919,50 @@
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:8">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="24">
         <v>9888882626</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="25" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" ht="15.5" spans="1:8">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="24">
         <v>9888882626</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="25" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1861,14 +1988,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="13.2909090909091" customWidth="1"/>
-    <col min="2" max="2" width="27.5818181818182" customWidth="1"/>
-    <col min="3" max="3" width="12.4181818181818" customWidth="1"/>
-    <col min="4" max="4" width="12.7090909090909" customWidth="1"/>
-    <col min="5" max="5" width="29.7090909090909" customWidth="1"/>
-    <col min="6" max="6" width="8.67272727272727" customWidth="1"/>
-    <col min="7" max="7" width="45.5727272727273" customWidth="1"/>
-    <col min="8" max="1025" width="8.67272727272727" customWidth="1"/>
+    <col min="1" max="1" width="13.2727272727273" customWidth="1"/>
+    <col min="2" max="2" width="27.5454545454545" customWidth="1"/>
+    <col min="3" max="3" width="12.4545454545455" customWidth="1"/>
+    <col min="4" max="4" width="12.7272727272727" customWidth="1"/>
+    <col min="5" max="5" width="29.7272727272727" customWidth="1"/>
+    <col min="6" max="6" width="8.63636363636364" customWidth="1"/>
+    <col min="7" max="7" width="45.5454545454545" customWidth="1"/>
+    <col min="8" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1895,48 +2022,48 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="10" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="10" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1966,61 +2093,61 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="14.8636363636364" customWidth="1"/>
-    <col min="2" max="3" width="15.2909090909091" customWidth="1"/>
-    <col min="4" max="4" width="27.4181818181818" customWidth="1"/>
-    <col min="5" max="5" width="16.5727272727273" customWidth="1"/>
-    <col min="6" max="1025" width="8.67272727272727" customWidth="1"/>
+    <col min="1" max="1" width="14.8181818181818" customWidth="1"/>
+    <col min="2" max="3" width="15.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="27.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="16.5454545454545" customWidth="1"/>
+    <col min="6" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="23" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="10" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="10" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2042,7 +2169,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1025" width="8.67272727272727" customWidth="1"/>
+    <col min="1" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2068,16 +2195,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="9.70909090909091" customWidth="1"/>
-    <col min="2" max="2" width="38.7" customWidth="1"/>
+    <col min="1" max="1" width="9.72727272727273" customWidth="1"/>
+    <col min="2" max="2" width="38.7272727272727" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="9.41818181818182" customWidth="1"/>
+    <col min="4" max="4" width="9.45454545454546" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="16.7090909090909" customWidth="1"/>
-    <col min="8" max="8" width="16.8636363636364" customWidth="1"/>
-    <col min="9" max="9" width="16.1363636363636" customWidth="1"/>
-    <col min="10" max="1025" width="8.67272727272727" customWidth="1"/>
+    <col min="7" max="7" width="16.7272727272727" customWidth="1"/>
+    <col min="8" max="8" width="16.9090909090909" customWidth="1"/>
+    <col min="9" max="9" width="16.1818181818182" customWidth="1"/>
+    <col min="10" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2095,30 +2222,30 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="10" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2140,26 +2267,39 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1" width="20.5727272727273" customWidth="1"/>
-    <col min="2" max="2" width="19.3090909090909" customWidth="1"/>
-    <col min="3" max="6" width="21.8181818181818" customWidth="1"/>
-    <col min="7" max="7" width="11.9363636363636" customWidth="1"/>
-    <col min="8" max="8" width="18.4727272727273" customWidth="1"/>
-    <col min="9" max="16" width="20.8272727272727" customWidth="1"/>
-    <col min="17" max="17" width="18.1818181818182" customWidth="1"/>
-    <col min="18" max="18" width="17.8181818181818" customWidth="1"/>
-    <col min="19" max="1027" width="8.67272727272727" customWidth="1"/>
+    <col min="1" max="1" width="20.5454545454545" customWidth="1"/>
+    <col min="2" max="2" width="19.2727272727273" customWidth="1"/>
+    <col min="3" max="3" width="51.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="30.7272727272727" customWidth="1"/>
+    <col min="5" max="6" width="21.8181818181818" customWidth="1"/>
+    <col min="7" max="7" width="11.9090909090909" customWidth="1"/>
+    <col min="8" max="8" width="18.4545454545455" customWidth="1"/>
+    <col min="9" max="12" width="20.8181818181818" customWidth="1"/>
+    <col min="13" max="13" width="18" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
+    <col min="15" max="15" width="10" customWidth="1"/>
+    <col min="16" max="16" width="14.9090909090909" customWidth="1"/>
+    <col min="17" max="17" width="16" customWidth="1"/>
+    <col min="18" max="18" width="18.5454545454545" customWidth="1"/>
+    <col min="19" max="19" width="10.8181818181818" customWidth="1"/>
+    <col min="20" max="20" width="10.3636363636364" customWidth="1"/>
+    <col min="21" max="23" width="8.63636363636364" customWidth="1"/>
+    <col min="24" max="24" width="11.3272727272727" customWidth="1"/>
+    <col min="25" max="25" width="8.63636363636364" customWidth="1"/>
+    <col min="26" max="26" width="15.1" customWidth="1"/>
+    <col min="27" max="27" width="10.2818181818182" customWidth="1"/>
+    <col min="28" max="1029" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2181,100 +2321,210 @@
       <c r="G1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="12" t="s">
         <v>103</v>
       </c>
+      <c r="T1" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="U1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="W1" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y1" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z1" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA1" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB1" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC1" s="17" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="2" spans="1:18">
-      <c r="A2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" s="6">
+    <row r="2" spans="1:29">
+      <c r="A2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="7">
         <v>9717254315</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="H2" s="8" t="s">
+      <c r="G2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="J2" s="10">
+      <c r="I2" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="13">
         <v>2345</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="R2" s="8" t="s">
+      <c r="K2" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="U2" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="V2" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="W2" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="X2" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y2" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z2" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA2" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB2" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC2" s="19" t="s">
         <v>91</v>
       </c>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+    </row>
+    <row r="7" spans="20:20">
+      <c r="T7" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" display="demo@yahooo.com"/>
+    <hyperlink ref="M2" r:id="rId1" display="demo@yahooo.com"/>
     <hyperlink ref="C2" r:id="rId2" display="https://testingxperts-5d-dev-ed.develop.my.salesforce.com"/>
+    <hyperlink ref="C3" r:id="rId3" display="https://testingxperts61-dev-ed.develop.my.salesforce.com"/>
+    <hyperlink ref="E3" r:id="rId4" display="Sharma@123#&amp;"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Adding ss module 25th latest
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11440" tabRatio="500" firstSheet="4" activeTab="6"/>
+    <workbookView windowWidth="19200" windowHeight="6800" tabRatio="500" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="WebTestData" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,25 @@
     <sheet name="Salesforce" sheetId="7" r:id="rId7"/>
     <sheet name="SalesforceLogin" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="147">
   <si>
     <t>TestData</t>
   </si>
@@ -353,6 +366,24 @@
     <t>Department</t>
   </si>
   <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>AccountName1</t>
+  </si>
+  <si>
+    <t>PhoneNumber1</t>
+  </si>
+  <si>
+    <t>FirstName1</t>
+  </si>
+  <si>
+    <t>LastName1</t>
+  </si>
+  <si>
     <t>TestData1</t>
   </si>
   <si>
@@ -420,6 +451,18 @@
   </si>
   <si>
     <t>Sales</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>TX_Nitu</t>
+  </si>
+  <si>
+    <t>Shruthi</t>
+  </si>
+  <si>
+    <t>Dharnaik</t>
   </si>
   <si>
     <t>https://testingxperts61-dev-ed.develop.my.salesforce.com</t>
@@ -437,14 +480,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -472,12 +515,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -512,6 +549,21 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -523,6 +575,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -533,66 +601,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -606,9 +630,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -616,21 +640,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -645,13 +654,41 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -684,181 +721,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -896,6 +927,19 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -903,19 +947,6 @@
         <color auto="1"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -950,26 +981,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -998,30 +1029,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1033,6 +1040,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1050,233 +1081,233 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="48" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="48" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="6" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="48" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="48" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="6" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="48" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1619,30 +1650,30 @@
       <selection activeCell="A1" sqref="G2 F10 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="14.8203125" customWidth="1"/>
-    <col min="2" max="3" width="15.2734375" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" customWidth="1"/>
-    <col min="6" max="6" width="10.8203125" customWidth="1"/>
-    <col min="7" max="7" width="28.1796875" customWidth="1"/>
-    <col min="8" max="8" width="26.2734375" customWidth="1"/>
-    <col min="9" max="9" width="10.09375" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" customWidth="1"/>
-    <col min="11" max="13" width="8.6328125" customWidth="1"/>
-    <col min="14" max="14" width="12.7265625" customWidth="1"/>
-    <col min="15" max="15" width="21.1796875" customWidth="1"/>
-    <col min="16" max="16" width="8.6328125" customWidth="1"/>
-    <col min="17" max="17" width="12.2734375" customWidth="1"/>
-    <col min="18" max="18" width="26.2734375" customWidth="1"/>
-    <col min="19" max="19" width="19.7265625" customWidth="1"/>
-    <col min="20" max="20" width="15.546875" customWidth="1"/>
-    <col min="21" max="21" width="14.8203125" customWidth="1"/>
-    <col min="22" max="22" width="18.7265625" customWidth="1"/>
-    <col min="23" max="23" width="21.1796875" customWidth="1"/>
-    <col min="24" max="24" width="32.2734375" customWidth="1"/>
-    <col min="25" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="14.8181818181818" customWidth="1"/>
+    <col min="2" max="3" width="15.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="27.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="9.45454545454546" customWidth="1"/>
+    <col min="6" max="6" width="10.8181818181818" customWidth="1"/>
+    <col min="7" max="7" width="28.1818181818182" customWidth="1"/>
+    <col min="8" max="8" width="26.2727272727273" customWidth="1"/>
+    <col min="9" max="9" width="10.0909090909091" customWidth="1"/>
+    <col min="10" max="10" width="9.72727272727273" customWidth="1"/>
+    <col min="11" max="13" width="8.63636363636364" customWidth="1"/>
+    <col min="14" max="14" width="12.7272727272727" customWidth="1"/>
+    <col min="15" max="15" width="21.1818181818182" customWidth="1"/>
+    <col min="16" max="16" width="8.63636363636364" customWidth="1"/>
+    <col min="17" max="17" width="12.2727272727273" customWidth="1"/>
+    <col min="18" max="18" width="26.2727272727273" customWidth="1"/>
+    <col min="19" max="19" width="19.7272727272727" customWidth="1"/>
+    <col min="20" max="20" width="15.5454545454545" customWidth="1"/>
+    <col min="21" max="21" width="14.8181818181818" customWidth="1"/>
+    <col min="22" max="22" width="18.7272727272727" customWidth="1"/>
+    <col min="23" max="23" width="21.1818181818182" customWidth="1"/>
+    <col min="24" max="24" width="32.2727272727273" customWidth="1"/>
+    <col min="25" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -1720,140 +1751,140 @@
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="V2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="W2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="X2" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E3" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6" t="s">
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="X3" s="10" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1873,15 +1904,15 @@
       <selection activeCell="A2" sqref="G2 F10 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="32.2734375" customWidth="1"/>
-    <col min="4" max="4" width="12.546875" customWidth="1"/>
-    <col min="5" max="7" width="8.6328125" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" customWidth="1"/>
-    <col min="9" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="9.72727272727273" customWidth="1"/>
+    <col min="2" max="2" width="12.4545454545455" customWidth="1"/>
+    <col min="3" max="3" width="32.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="12.5454545454545" customWidth="1"/>
+    <col min="5" max="7" width="8.63636363636364" customWidth="1"/>
+    <col min="8" max="8" width="17.7272727272727" customWidth="1"/>
+    <col min="9" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1910,8 +1941,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" ht="14.8" spans="1:8">
-      <c r="A2" s="6" t="s">
+    <row r="2" ht="15.5" spans="1:8">
+      <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="26">
@@ -1936,8 +1967,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" ht="14.8" spans="1:8">
-      <c r="A3" s="6" t="s">
+    <row r="3" ht="15.5" spans="1:8">
+      <c r="A3" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B3" s="26">
@@ -1978,16 +2009,16 @@
       <selection activeCell="E1" sqref="G2 F10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="13.2734375" customWidth="1"/>
-    <col min="2" max="2" width="27.546875" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" customWidth="1"/>
-    <col min="5" max="5" width="29.7265625" customWidth="1"/>
-    <col min="6" max="6" width="8.6328125" customWidth="1"/>
-    <col min="7" max="7" width="45.546875" customWidth="1"/>
-    <col min="8" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="13.2727272727273" customWidth="1"/>
+    <col min="2" max="2" width="27.5454545454545" customWidth="1"/>
+    <col min="3" max="3" width="12.4545454545455" customWidth="1"/>
+    <col min="4" max="4" width="12.7272727272727" customWidth="1"/>
+    <col min="5" max="5" width="29.7272727272727" customWidth="1"/>
+    <col min="6" max="6" width="8.63636363636364" customWidth="1"/>
+    <col min="7" max="7" width="45.5454545454545" customWidth="1"/>
+    <col min="8" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2014,48 +2045,48 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>62</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="10" t="s">
         <v>65</v>
       </c>
       <c r="E2" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="10" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="10" t="s">
         <v>69</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="10" t="s">
         <v>70</v>
       </c>
       <c r="E3" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="10" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2083,13 +2114,13 @@
       <selection activeCell="C8" sqref="G2 F10 C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="14.8203125" customWidth="1"/>
-    <col min="2" max="3" width="15.2734375" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.546875" customWidth="1"/>
-    <col min="6" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="14.8181818181818" customWidth="1"/>
+    <col min="2" max="3" width="15.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="27.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="16.5454545454545" customWidth="1"/>
+    <col min="6" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2110,36 +2141,36 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="10" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="10" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2159,9 +2190,9 @@
       <selection activeCell="C7" sqref="G2 F10 C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2185,18 +2216,18 @@
       <selection activeCell="E1" sqref="G2 F10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" customWidth="1"/>
-    <col min="2" max="2" width="38.7265625" customWidth="1"/>
+    <col min="1" max="1" width="9.72727272727273" customWidth="1"/>
+    <col min="2" max="2" width="38.7272727272727" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" customWidth="1"/>
+    <col min="4" max="4" width="9.45454545454546" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="16.90625" customWidth="1"/>
-    <col min="9" max="9" width="16.1796875" customWidth="1"/>
-    <col min="10" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="7" max="7" width="16.7272727272727" customWidth="1"/>
+    <col min="8" max="8" width="16.9090909090909" customWidth="1"/>
+    <col min="9" max="9" width="16.1818181818182" customWidth="1"/>
+    <col min="10" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2214,7 +2245,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="23" t="s">
@@ -2223,12 +2254,12 @@
       <c r="C2" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="10" t="s">
         <v>88</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -2237,7 +2268,7 @@
       <c r="C3" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="10" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2259,39 +2290,43 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AA7"/>
+  <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1" width="20.546875" customWidth="1"/>
-    <col min="2" max="2" width="19.2734375" customWidth="1"/>
-    <col min="3" max="3" width="51.2734375" customWidth="1"/>
-    <col min="4" max="4" width="30.7265625" customWidth="1"/>
-    <col min="5" max="6" width="21.8203125" customWidth="1"/>
-    <col min="7" max="7" width="11.90625" customWidth="1"/>
-    <col min="8" max="8" width="18.453125" customWidth="1"/>
-    <col min="9" max="12" width="20.8203125" customWidth="1"/>
+    <col min="1" max="1" width="20.5454545454545" customWidth="1"/>
+    <col min="2" max="2" width="19.2727272727273" customWidth="1"/>
+    <col min="3" max="3" width="51.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="30.7272727272727" customWidth="1"/>
+    <col min="5" max="6" width="21.8181818181818" customWidth="1"/>
+    <col min="7" max="7" width="11.9090909090909" customWidth="1"/>
+    <col min="8" max="8" width="18.4545454545455" customWidth="1"/>
+    <col min="9" max="12" width="20.8181818181818" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
     <col min="14" max="14" width="9" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
-    <col min="16" max="16" width="14.90625" customWidth="1"/>
+    <col min="16" max="16" width="14.9090909090909" customWidth="1"/>
     <col min="17" max="17" width="16" customWidth="1"/>
-    <col min="18" max="18" width="18.546875" customWidth="1"/>
-    <col min="19" max="19" width="10.8203125" customWidth="1"/>
-    <col min="20" max="20" width="10.3671875" customWidth="1"/>
-    <col min="21" max="23" width="8.6328125" customWidth="1"/>
-    <col min="24" max="24" width="11.328125" customWidth="1"/>
-    <col min="25" max="25" width="8.6328125" customWidth="1"/>
-    <col min="26" max="26" width="15.1015625" customWidth="1"/>
-    <col min="27" max="27" width="10.28125" customWidth="1"/>
-    <col min="28" max="1029" width="8.6328125" customWidth="1"/>
+    <col min="18" max="18" width="18.5454545454545" customWidth="1"/>
+    <col min="19" max="19" width="10.8181818181818" customWidth="1"/>
+    <col min="20" max="20" width="10.3636363636364" customWidth="1"/>
+    <col min="21" max="23" width="8.63636363636364" customWidth="1"/>
+    <col min="24" max="24" width="11.3272727272727" customWidth="1"/>
+    <col min="25" max="25" width="8.63636363636364" customWidth="1"/>
+    <col min="26" max="26" width="15.1" customWidth="1"/>
+    <col min="27" max="27" width="10.2818181818182" customWidth="1"/>
+    <col min="28" max="30" width="8.63636363636364" customWidth="1"/>
+    <col min="31" max="31" width="16" customWidth="1"/>
+    <col min="32" max="32" width="8.63636363636364" customWidth="1"/>
+    <col min="33" max="33" width="13" customWidth="1"/>
+    <col min="34" max="1029" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:33">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2310,194 +2345,236 @@
       <c r="F1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="T1" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="U1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="V1" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="W1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="X1" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Y1" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="Z1" s="18" t="s">
+      <c r="Z1" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AA1" s="17" t="s">
         <v>109</v>
       </c>
+      <c r="AB1" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC1" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="AD1" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AF1" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG1" s="17" t="s">
+        <v>115</v>
+      </c>
     </row>
-    <row r="2" spans="1:27">
-      <c r="A2" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F2" s="5">
+    <row r="2" spans="1:33">
+      <c r="A2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="7">
         <v>9717254315</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="H2" s="11" t="s">
+      <c r="G2" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="J2" s="12">
+      <c r="I2" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="J2" s="13">
         <v>2345</v>
       </c>
-      <c r="K2" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>118</v>
+      <c r="K2" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>124</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N2" s="15" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="O2" s="16"/>
       <c r="P2" s="16" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="Q2" s="16" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="R2" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="U2" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="V2" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="W2" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="X2" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="Y2" s="20" t="s">
+      <c r="S2" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="Z2" s="20" t="s">
+      <c r="T2" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="AA2" s="20" t="s">
+      <c r="U2" s="19" t="s">
         <v>132</v>
       </c>
+      <c r="V2" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="W2" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="X2" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y2" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z2" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA2" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB2" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC2" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE2" s="21">
+        <v>9717254315</v>
+      </c>
+      <c r="AF2" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="AG2" s="19" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="3" spans="1:27">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:33">
+      <c r="A3" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="O3" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="22"/>
-      <c r="V3" s="22"/>
-      <c r="W3" s="22"/>
-      <c r="X3" s="22"/>
-      <c r="Y3" s="22"/>
-      <c r="Z3" s="22"/>
-      <c r="AA3" s="22"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="22"/>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="22"/>
+      <c r="AE3" s="22"/>
+      <c r="AF3" s="22"/>
+      <c r="AG3" s="22"/>
     </row>
     <row r="7" spans="20:20">
-      <c r="T7" s="6"/>
+      <c r="T7" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2521,7 +2598,7 @@
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
commit for Forecasting Module review comment resolve
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SalesforceAutomation_24thApril\SalesforceAutomation\src\test\resources\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3084A30-76DC-4484-8717-35484526B225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="11440" tabRatio="500" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="WebTestData" sheetId="1" r:id="rId1"/>
@@ -27,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="137">
   <si>
     <t>TestData</t>
   </si>
@@ -344,6 +338,21 @@
     <t>FieldValue</t>
   </si>
   <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>n_username</t>
+  </si>
+  <si>
+    <t>Nickname</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
     <t>TestData1</t>
   </si>
   <si>
@@ -374,6 +383,9 @@
     <t>demo@yahooo.com</t>
   </si>
   <si>
+    <t>Sharma</t>
+  </si>
+  <si>
     <t>YearABC</t>
   </si>
   <si>
@@ -389,23 +401,50 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Nisha</t>
+  </si>
+  <si>
+    <t>nsharma</t>
+  </si>
+  <si>
+    <t>ynitu913@gmail.com</t>
+  </si>
+  <si>
+    <t>NiaSharma</t>
+  </si>
+  <si>
+    <t>Nia</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>https://testingxperts61-dev-ed.develop.my.salesforce.com</t>
+  </si>
+  <si>
+    <t>anil53756@gmail.com</t>
+  </si>
+  <si>
+    <t>Sharma@123#&amp;</t>
+  </si>
+  <si>
     <t>Hyderabad</t>
-  </si>
-  <si>
-    <t>https://testing-f5-dev-ed.develop.my.salesforce.com</t>
-  </si>
-  <si>
-    <t>barwalrohitthakur@gmail.com</t>
-  </si>
-  <si>
-    <t>Trigma@789</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -433,6 +472,12 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -444,8 +489,151 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,12 +654,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF8EB4E3"/>
         <bgColor rgb="FF95B3D7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -498,6 +872,19 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top style="thin">
         <color auto="1"/>
@@ -505,19 +892,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -551,40 +925,325 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="48" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="48" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="48" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="48" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="48" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -657,9 +1316,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -917,41 +1573,41 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="G2 F10 A1"/>
+      <selection activeCell="A1" sqref="G2 F10 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" customWidth="1"/>
-    <col min="2" max="3" width="15.26953125" customWidth="1"/>
+    <col min="1" max="1" width="14.8203125" customWidth="1"/>
+    <col min="2" max="3" width="15.2734375" customWidth="1"/>
     <col min="4" max="4" width="27.453125" customWidth="1"/>
     <col min="5" max="5" width="9.453125" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" customWidth="1"/>
+    <col min="6" max="6" width="10.8203125" customWidth="1"/>
     <col min="7" max="7" width="28.1796875" customWidth="1"/>
-    <col min="8" max="8" width="26.26953125" customWidth="1"/>
-    <col min="9" max="9" width="10.08984375" customWidth="1"/>
+    <col min="8" max="8" width="26.2734375" customWidth="1"/>
+    <col min="9" max="9" width="10.09375" customWidth="1"/>
     <col min="10" max="10" width="9.7265625" customWidth="1"/>
     <col min="11" max="13" width="8.6328125" customWidth="1"/>
     <col min="14" max="14" width="12.7265625" customWidth="1"/>
     <col min="15" max="15" width="21.1796875" customWidth="1"/>
     <col min="16" max="16" width="8.6328125" customWidth="1"/>
-    <col min="17" max="17" width="12.26953125" customWidth="1"/>
-    <col min="18" max="18" width="26.26953125" customWidth="1"/>
+    <col min="17" max="17" width="12.2734375" customWidth="1"/>
+    <col min="18" max="18" width="26.2734375" customWidth="1"/>
     <col min="19" max="19" width="19.7265625" customWidth="1"/>
-    <col min="20" max="20" width="15.54296875" customWidth="1"/>
-    <col min="21" max="21" width="14.81640625" customWidth="1"/>
+    <col min="20" max="20" width="15.546875" customWidth="1"/>
+    <col min="21" max="21" width="14.8203125" customWidth="1"/>
     <col min="22" max="22" width="18.7265625" customWidth="1"/>
     <col min="23" max="23" width="21.1796875" customWidth="1"/>
-    <col min="24" max="24" width="32.26953125" customWidth="1"/>
+    <col min="24" max="24" width="32.2734375" customWidth="1"/>
     <col min="25" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1030,163 +1686,165 @@
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="P2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="Q2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="R2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="S2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="10" t="s">
+      <c r="T2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="U2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="10" t="s">
+      <c r="V2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="10" t="s">
+      <c r="W2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="10" t="s">
+      <c r="X2" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10" t="s">
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="Q3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="R3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="S3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="T3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="U3" s="10" t="s">
+      <c r="U3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="10" t="s">
+      <c r="V3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="W3" s="10" t="s">
+      <c r="W3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="10" t="s">
+      <c r="X3" s="6" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="G2 F10 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="9.7265625" customWidth="1"/>
     <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="32.26953125" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" customWidth="1"/>
+    <col min="3" max="3" width="32.2734375" customWidth="1"/>
+    <col min="4" max="4" width="12.546875" customWidth="1"/>
     <col min="5" max="7" width="8.6328125" customWidth="1"/>
     <col min="8" max="8" width="17.7265625" customWidth="1"/>
     <col min="9" max="1025" width="8.6328125" customWidth="1"/>
@@ -1218,8 +1876,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.5">
-      <c r="A2" s="10" t="s">
+    <row r="2" ht="14.8" spans="1:8">
+      <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="20">
@@ -1244,8 +1902,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.5">
-      <c r="A3" s="10" t="s">
+    <row r="3" ht="14.8" spans="1:8">
+      <c r="A3" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B3" s="20">
@@ -1268,31 +1926,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="H2" r:id="rId1" display="w@maxbupa.com"/>
+    <hyperlink ref="H3" r:id="rId1" display="w@maxbupa.com"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="G2 F10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" customWidth="1"/>
-    <col min="2" max="2" width="27.54296875" customWidth="1"/>
+    <col min="1" max="1" width="13.2734375" customWidth="1"/>
+    <col min="2" max="2" width="27.546875" customWidth="1"/>
     <col min="3" max="3" width="12.453125" customWidth="1"/>
     <col min="4" max="4" width="12.7265625" customWidth="1"/>
     <col min="5" max="5" width="29.7265625" customWidth="1"/>
     <col min="6" max="6" width="8.6328125" customWidth="1"/>
-    <col min="7" max="7" width="45.54296875" customWidth="1"/>
+    <col min="7" max="7" width="45.546875" customWidth="1"/>
     <col min="8" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1320,79 +1980,81 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="6" t="s">
         <v>62</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="6" t="s">
         <v>65</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>69</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="6" t="s">
         <v>70</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="6" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="D3" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="E3" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.amazon.in/"/>
+    <hyperlink ref="D2" r:id="rId2" display="Damco@124"/>
+    <hyperlink ref="E2" r:id="rId3" display="XYZTestr@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.amazon.in/"/>
+    <hyperlink ref="D3" r:id="rId2" display="Damco@123"/>
+    <hyperlink ref="E3" r:id="rId3" display="XYZTestr@gmail.com"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="G2 F10 C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" customWidth="1"/>
-    <col min="2" max="3" width="15.26953125" customWidth="1"/>
+    <col min="1" max="1" width="14.8203125" customWidth="1"/>
+    <col min="2" max="3" width="15.2734375" customWidth="1"/>
     <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" customWidth="1"/>
+    <col min="5" max="5" width="16.546875" customWidth="1"/>
     <col min="6" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1414,54 +2076,56 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="6" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="G2 F10 C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
@@ -1472,20 +2136,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="G2 F10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="9.7265625" customWidth="1"/>
     <col min="2" max="2" width="38.7265625" customWidth="1"/>
@@ -1514,7 +2180,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="6" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -1523,12 +2189,12 @@
       <c r="C2" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="6" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>88</v>
       </c>
       <c r="B3" s="17" t="s">
@@ -1537,55 +2203,61 @@
       <c r="C3" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="6" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="C3" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="D3" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://release.getcheddarup.com/login/"/>
+    <hyperlink ref="C2" r:id="rId2" display="sarahsmith@example.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="tester1"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://release.getcheddarup.com/login/"/>
+    <hyperlink ref="C3" r:id="rId2" display="sarahsmith@example.com"/>
+    <hyperlink ref="D3" r:id="rId3" display="tester123"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:U10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" customWidth="1"/>
-    <col min="2" max="2" width="19.26953125" customWidth="1"/>
-    <col min="3" max="3" width="51.26953125" customWidth="1"/>
+    <col min="1" max="1" width="20.546875" customWidth="1"/>
+    <col min="2" max="2" width="19.2734375" customWidth="1"/>
+    <col min="3" max="3" width="51.2734375" customWidth="1"/>
     <col min="4" max="4" width="30.7265625" customWidth="1"/>
-    <col min="5" max="6" width="21.81640625" customWidth="1"/>
+    <col min="5" max="6" width="21.8203125" customWidth="1"/>
     <col min="7" max="7" width="11.90625" customWidth="1"/>
     <col min="8" max="8" width="18.453125" customWidth="1"/>
-    <col min="9" max="12" width="20.81640625" customWidth="1"/>
+    <col min="9" max="12" width="20.8203125" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="11.54296875" hidden="1"/>
-    <col min="15" max="15" width="9" customWidth="1"/>
-    <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="17" max="17" width="14.90625" customWidth="1"/>
-    <col min="18" max="18" width="16" customWidth="1"/>
-    <col min="19" max="19" width="18.54296875" customWidth="1"/>
-    <col min="20" max="20" width="10.81640625" customWidth="1"/>
-    <col min="21" max="21" width="10.36328125" customWidth="1"/>
-    <col min="22" max="1031" width="8.6328125" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
+    <col min="15" max="15" width="10" customWidth="1"/>
+    <col min="16" max="16" width="14.90625" customWidth="1"/>
+    <col min="17" max="17" width="16" customWidth="1"/>
+    <col min="18" max="18" width="18.546875" customWidth="1"/>
+    <col min="19" max="19" width="10.8203125" customWidth="1"/>
+    <col min="20" max="20" width="10.3671875" customWidth="1"/>
+    <col min="21" max="23" width="8.6328125" customWidth="1"/>
+    <col min="24" max="24" width="11.328125" customWidth="1"/>
+    <col min="25" max="25" width="8.6328125" customWidth="1"/>
+    <col min="26" max="26" width="15.1015625" customWidth="1"/>
+    <col min="27" max="27" width="10.28125" customWidth="1"/>
+    <col min="28" max="1029" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:27">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1604,173 +2276,220 @@
       <c r="F1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="12"/>
-      <c r="O1" s="3" t="s">
+      <c r="N1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="O1" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="P1" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="Q1" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="R1" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="S1" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="T1" s="13" t="s">
         <v>104</v>
       </c>
+      <c r="U1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="W1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z1" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F2" s="7">
+    <row r="2" spans="1:27">
+      <c r="A2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="5">
         <v>9717254315</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="J2" s="13">
+      <c r="I2" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" s="12">
         <v>2345</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>113</v>
+      <c r="K2" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>118</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="N2" s="14"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="U2" s="10" t="s">
         <v>119</v>
       </c>
+      <c r="N2" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="X2" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA2" s="11" t="s">
+        <v>132</v>
+      </c>
     </row>
-    <row r="3" spans="1:21">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:27">
+      <c r="A3" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="P3" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
     </row>
-    <row r="10" spans="1:21">
-      <c r="U10" s="10"/>
+    <row r="7" spans="20:20">
+      <c r="T7" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{22CA66F3-0571-4BA4-AC8E-057A790A013A}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{9CAA5FC9-3B01-4D87-B383-6C1D2C5993B5}"/>
+    <hyperlink ref="M2" r:id="rId1" display="demo@yahooo.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="https://testingxperts-5d-dev-ed.develop.my.salesforce.com"/>
+    <hyperlink ref="C3" r:id="rId3" display="https://testingxperts61-dev-ed.develop.my.salesforce.com"/>
+    <hyperlink ref="E3" r:id="rId4" display="Sharma@123#&amp;"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
saving service support module.
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11440" tabRatio="500" firstSheet="4" activeTab="6"/>
+    <workbookView windowWidth="19200" windowHeight="6800" tabRatio="500" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="WebTestData" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,25 @@
     <sheet name="Salesforce" sheetId="7" r:id="rId7"/>
     <sheet name="SalesforceLogin" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="141">
   <si>
     <t>TestData</t>
   </si>
@@ -353,6 +366,12 @@
     <t>Department</t>
   </si>
   <si>
+    <t>InReviewStatus</t>
+  </si>
+  <si>
+    <t>ApprovedStatus</t>
+  </si>
+  <si>
     <t>TestData1</t>
   </si>
   <si>
@@ -420,6 +439,12 @@
   </si>
   <si>
     <t>Sales</t>
+  </si>
+  <si>
+    <t>In Review</t>
+  </si>
+  <si>
+    <t>Approved</t>
   </si>
   <si>
     <t>https://testingxperts61-dev-ed.develop.my.salesforce.com</t>
@@ -437,11 +462,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
@@ -497,9 +522,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -512,38 +537,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -558,10 +553,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -572,8 +584,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -581,7 +594,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -602,11 +623,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -617,19 +644,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -666,67 +691,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -738,13 +835,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -756,91 +865,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -872,6 +897,19 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -879,19 +917,6 @@
         <color auto="1"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -926,17 +951,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -956,30 +999,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -990,6 +1009,21 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1014,235 +1048,227 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="48" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="48" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="6" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="48" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="6" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="48" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1585,30 +1611,30 @@
       <selection activeCell="A1" sqref="G2 F10 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="14.8203125" customWidth="1"/>
-    <col min="2" max="3" width="15.2734375" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" customWidth="1"/>
-    <col min="6" max="6" width="10.8203125" customWidth="1"/>
-    <col min="7" max="7" width="28.1796875" customWidth="1"/>
-    <col min="8" max="8" width="26.2734375" customWidth="1"/>
-    <col min="9" max="9" width="10.09375" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" customWidth="1"/>
-    <col min="11" max="13" width="8.6328125" customWidth="1"/>
-    <col min="14" max="14" width="12.7265625" customWidth="1"/>
-    <col min="15" max="15" width="21.1796875" customWidth="1"/>
-    <col min="16" max="16" width="8.6328125" customWidth="1"/>
-    <col min="17" max="17" width="12.2734375" customWidth="1"/>
-    <col min="18" max="18" width="26.2734375" customWidth="1"/>
-    <col min="19" max="19" width="19.7265625" customWidth="1"/>
-    <col min="20" max="20" width="15.546875" customWidth="1"/>
-    <col min="21" max="21" width="14.8203125" customWidth="1"/>
-    <col min="22" max="22" width="18.7265625" customWidth="1"/>
-    <col min="23" max="23" width="21.1796875" customWidth="1"/>
-    <col min="24" max="24" width="32.2734375" customWidth="1"/>
-    <col min="25" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="14.8181818181818" customWidth="1"/>
+    <col min="2" max="3" width="15.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="27.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="9.45454545454546" customWidth="1"/>
+    <col min="6" max="6" width="10.8181818181818" customWidth="1"/>
+    <col min="7" max="7" width="28.1818181818182" customWidth="1"/>
+    <col min="8" max="8" width="26.2727272727273" customWidth="1"/>
+    <col min="9" max="9" width="10.0909090909091" customWidth="1"/>
+    <col min="10" max="10" width="9.72727272727273" customWidth="1"/>
+    <col min="11" max="13" width="8.63636363636364" customWidth="1"/>
+    <col min="14" max="14" width="12.7272727272727" customWidth="1"/>
+    <col min="15" max="15" width="21.1818181818182" customWidth="1"/>
+    <col min="16" max="16" width="8.63636363636364" customWidth="1"/>
+    <col min="17" max="17" width="12.2727272727273" customWidth="1"/>
+    <col min="18" max="18" width="26.2727272727273" customWidth="1"/>
+    <col min="19" max="19" width="19.7272727272727" customWidth="1"/>
+    <col min="20" max="20" width="15.5454545454545" customWidth="1"/>
+    <col min="21" max="21" width="14.8181818181818" customWidth="1"/>
+    <col min="22" max="22" width="18.7272727272727" customWidth="1"/>
+    <col min="23" max="23" width="21.1818181818182" customWidth="1"/>
+    <col min="24" max="24" width="32.2727272727273" customWidth="1"/>
+    <col min="25" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -1686,140 +1712,140 @@
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="V2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="W2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="X2" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6" t="s">
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="X3" s="10" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1839,15 +1865,15 @@
       <selection activeCell="A2" sqref="G2 F10 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="32.2734375" customWidth="1"/>
-    <col min="4" max="4" width="12.546875" customWidth="1"/>
-    <col min="5" max="7" width="8.6328125" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" customWidth="1"/>
-    <col min="9" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="9.72727272727273" customWidth="1"/>
+    <col min="2" max="2" width="12.4545454545455" customWidth="1"/>
+    <col min="3" max="3" width="32.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="12.5454545454545" customWidth="1"/>
+    <col min="5" max="7" width="8.63636363636364" customWidth="1"/>
+    <col min="8" max="8" width="17.7272727272727" customWidth="1"/>
+    <col min="9" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1876,51 +1902,51 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" ht="14.8" spans="1:8">
-      <c r="A2" s="6" t="s">
+    <row r="2" ht="15.5" spans="1:8">
+      <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="21">
         <v>9888882626</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" ht="14.8" spans="1:8">
-      <c r="A3" s="6" t="s">
+    <row r="3" ht="15.5" spans="1:8">
+      <c r="A3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="21">
         <v>9888882626</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="22" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1944,16 +1970,16 @@
       <selection activeCell="E1" sqref="G2 F10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="13.2734375" customWidth="1"/>
-    <col min="2" max="2" width="27.546875" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" customWidth="1"/>
-    <col min="5" max="5" width="29.7265625" customWidth="1"/>
-    <col min="6" max="6" width="8.6328125" customWidth="1"/>
-    <col min="7" max="7" width="45.546875" customWidth="1"/>
-    <col min="8" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="13.2727272727273" customWidth="1"/>
+    <col min="2" max="2" width="27.5454545454545" customWidth="1"/>
+    <col min="3" max="3" width="12.4545454545455" customWidth="1"/>
+    <col min="4" max="4" width="12.7272727272727" customWidth="1"/>
+    <col min="5" max="5" width="29.7272727272727" customWidth="1"/>
+    <col min="6" max="6" width="8.63636363636364" customWidth="1"/>
+    <col min="7" max="7" width="45.5454545454545" customWidth="1"/>
+    <col min="8" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1980,48 +2006,48 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="10" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="10" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2049,63 +2075,63 @@
       <selection activeCell="C8" sqref="G2 F10 C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="14.8203125" customWidth="1"/>
-    <col min="2" max="3" width="15.2734375" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.546875" customWidth="1"/>
-    <col min="6" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="14.8181818181818" customWidth="1"/>
+    <col min="2" max="3" width="15.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="27.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="16.5454545454545" customWidth="1"/>
+    <col min="6" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="10" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="10" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2125,9 +2151,9 @@
       <selection activeCell="C7" sqref="G2 F10 C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2151,18 +2177,18 @@
       <selection activeCell="E1" sqref="G2 F10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" customWidth="1"/>
-    <col min="2" max="2" width="38.7265625" customWidth="1"/>
+    <col min="1" max="1" width="9.72727272727273" customWidth="1"/>
+    <col min="2" max="2" width="38.7272727272727" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" customWidth="1"/>
+    <col min="4" max="4" width="9.45454545454546" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="16.90625" customWidth="1"/>
-    <col min="9" max="9" width="16.1796875" customWidth="1"/>
-    <col min="10" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="7" max="7" width="16.7272727272727" customWidth="1"/>
+    <col min="8" max="8" width="16.9090909090909" customWidth="1"/>
+    <col min="9" max="9" width="16.1818181818182" customWidth="1"/>
+    <col min="10" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2180,30 +2206,30 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="10" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2225,39 +2251,41 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AA7"/>
+  <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA9"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1" width="20.546875" customWidth="1"/>
-    <col min="2" max="2" width="19.2734375" customWidth="1"/>
-    <col min="3" max="3" width="51.2734375" customWidth="1"/>
-    <col min="4" max="4" width="30.7265625" customWidth="1"/>
-    <col min="5" max="6" width="21.8203125" customWidth="1"/>
-    <col min="7" max="7" width="11.90625" customWidth="1"/>
-    <col min="8" max="8" width="18.453125" customWidth="1"/>
-    <col min="9" max="12" width="20.8203125" customWidth="1"/>
+    <col min="1" max="1" width="20.5454545454545" customWidth="1"/>
+    <col min="2" max="2" width="19.2727272727273" customWidth="1"/>
+    <col min="3" max="3" width="51.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="30.7272727272727" customWidth="1"/>
+    <col min="5" max="6" width="21.8181818181818" customWidth="1"/>
+    <col min="7" max="7" width="11.9090909090909" customWidth="1"/>
+    <col min="8" max="8" width="18.4545454545455" customWidth="1"/>
+    <col min="9" max="12" width="20.8181818181818" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
     <col min="14" max="14" width="9" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
-    <col min="16" max="16" width="14.90625" customWidth="1"/>
+    <col min="16" max="16" width="14.9090909090909" customWidth="1"/>
     <col min="17" max="17" width="16" customWidth="1"/>
-    <col min="18" max="18" width="18.546875" customWidth="1"/>
-    <col min="19" max="19" width="10.8203125" customWidth="1"/>
-    <col min="20" max="20" width="10.3671875" customWidth="1"/>
-    <col min="21" max="23" width="8.6328125" customWidth="1"/>
-    <col min="24" max="24" width="11.328125" customWidth="1"/>
-    <col min="25" max="25" width="8.6328125" customWidth="1"/>
-    <col min="26" max="26" width="15.1015625" customWidth="1"/>
-    <col min="27" max="27" width="10.28125" customWidth="1"/>
-    <col min="28" max="1029" width="8.6328125" customWidth="1"/>
+    <col min="18" max="18" width="18.5454545454545" customWidth="1"/>
+    <col min="19" max="19" width="10.8181818181818" customWidth="1"/>
+    <col min="20" max="20" width="10.3636363636364" customWidth="1"/>
+    <col min="21" max="23" width="8.63636363636364" customWidth="1"/>
+    <col min="24" max="24" width="11.3272727272727" customWidth="1"/>
+    <col min="25" max="25" width="8.63636363636364" customWidth="1"/>
+    <col min="26" max="26" width="15.1" customWidth="1"/>
+    <col min="27" max="27" width="10.2818181818182" customWidth="1"/>
+    <col min="28" max="28" width="21.2727272727273" customWidth="1"/>
+    <col min="29" max="29" width="16.4545454545455" customWidth="1"/>
+    <col min="30" max="1029" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2276,194 +2304,208 @@
       <c r="F1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="T1" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="U1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="V1" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="W1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="X1" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Y1" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="Z1" s="12" t="s">
         <v>108</v>
       </c>
       <c r="AA1" s="16" t="s">
         <v>109</v>
       </c>
+      <c r="AB1" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC1" s="12" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="2" spans="1:27">
-      <c r="A2" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    <row r="2" spans="1:29">
+      <c r="A2" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="5">
+      <c r="D2" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="7">
         <v>9717254315</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="H2" s="11" t="s">
+      <c r="G2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="J2" s="12">
+      <c r="I2" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="13">
         <v>2345</v>
       </c>
-      <c r="K2" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>118</v>
+      <c r="K2" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>120</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="N2" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="O2" s="9"/>
+      <c r="P2" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="Q2" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="R2" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="U2" s="11" t="s">
+      <c r="S2" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="T2" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="W2" s="11" t="s">
+      <c r="U2" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="X2" s="11" t="s">
+      <c r="V2" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="Y2" s="11" t="s">
+      <c r="W2" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="Z2" s="11" t="s">
+      <c r="X2" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="AA2" s="11" t="s">
+      <c r="Y2" s="9" t="s">
         <v>132</v>
       </c>
+      <c r="Z2" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>136</v>
+      </c>
     </row>
-    <row r="3" spans="1:27">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:29">
+      <c r="A3" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
       <c r="N3" s="15" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="O3" s="15" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="17"/>
+      <c r="AC3" s="17"/>
     </row>
     <row r="7" spans="20:20">
-      <c r="T7" s="6"/>
+      <c r="T7" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2487,7 +2529,7 @@
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
commiting the code for salesforce billing and marketing
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SalesforceAutomation_24thApril\SalesforceAutomation\src\test\resources\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C47667-F315-4232-9BB3-0BC9952D9621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="19200" windowHeight="6800" tabRatio="500" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="WebTestData" sheetId="1" r:id="rId1"/>
@@ -22,12 +16,25 @@
     <sheet name="Salesforce" sheetId="7" r:id="rId7"/>
     <sheet name="SalesforceLogin" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="137">
   <si>
     <t>TestData</t>
   </si>
@@ -344,6 +351,27 @@
     <t>FieldValue</t>
   </si>
   <si>
+    <t>ContactLastname1</t>
+  </si>
+  <si>
+    <t>ContactEmail1</t>
+  </si>
+  <si>
+    <t>ContactPhone1</t>
+  </si>
+  <si>
+    <t>AccountName1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Salutation1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ContactPhone2 </t>
+  </si>
+  <si>
+    <t>ContactLastName2</t>
+  </si>
+  <si>
     <t>TestData1</t>
   </si>
   <si>
@@ -374,6 +402,12 @@
     <t>demo@yahooo.com</t>
   </si>
   <si>
+    <t>Anil</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
     <t>YearABC</t>
   </si>
   <si>
@@ -383,35 +417,47 @@
     <t>Year1</t>
   </si>
   <si>
-    <t>Anil</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Singh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ns123@gmail.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NishuTX </t>
+  </si>
+  <si>
+    <t>Ms</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>https://testingxperts61-dev-ed.develop.my.salesforce.com</t>
+  </si>
+  <si>
+    <t>anil53756@gmail.com</t>
+  </si>
+  <si>
+    <t>Sharma@123#&amp;</t>
+  </si>
+  <si>
     <t>Hyderabad</t>
-  </si>
-  <si>
-    <t>https://testing-f5-dev-ed.develop.my.salesforce.com</t>
-  </si>
-  <si>
-    <t>barwalrohitthakur@gmail.com</t>
-  </si>
-  <si>
-    <t>Trigma@789</t>
-  </si>
-  <si>
-    <t>Qualification</t>
-  </si>
-  <si>
-    <t>Computer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -424,6 +470,13 @@
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
     <font>
       <u/>
@@ -450,8 +503,151 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -476,8 +672,194 @@
         <bgColor rgb="FF95B3D7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -557,40 +939,335 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="6" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="6" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -663,9 +1340,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -923,42 +1597,42 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="G2 F10 A1"/>
+      <selection activeCell="A1" sqref="G2 F10 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" customWidth="1"/>
-    <col min="2" max="3" width="15.26953125" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" customWidth="1"/>
-    <col min="7" max="7" width="28.1796875" customWidth="1"/>
-    <col min="8" max="8" width="26.26953125" customWidth="1"/>
-    <col min="9" max="9" width="10.08984375" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" customWidth="1"/>
-    <col min="11" max="13" width="8.6328125" customWidth="1"/>
-    <col min="14" max="14" width="12.7265625" customWidth="1"/>
-    <col min="15" max="15" width="21.1796875" customWidth="1"/>
-    <col min="16" max="16" width="8.6328125" customWidth="1"/>
-    <col min="17" max="17" width="12.26953125" customWidth="1"/>
-    <col min="18" max="18" width="26.26953125" customWidth="1"/>
-    <col min="19" max="19" width="19.7265625" customWidth="1"/>
-    <col min="20" max="20" width="15.54296875" customWidth="1"/>
-    <col min="21" max="21" width="14.81640625" customWidth="1"/>
-    <col min="22" max="22" width="18.7265625" customWidth="1"/>
-    <col min="23" max="23" width="21.1796875" customWidth="1"/>
-    <col min="24" max="24" width="32.26953125" customWidth="1"/>
-    <col min="25" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="14.8181818181818" customWidth="1"/>
+    <col min="2" max="3" width="15.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="27.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="9.45454545454546" customWidth="1"/>
+    <col min="6" max="6" width="10.8181818181818" customWidth="1"/>
+    <col min="7" max="7" width="28.1818181818182" customWidth="1"/>
+    <col min="8" max="8" width="26.2727272727273" customWidth="1"/>
+    <col min="9" max="9" width="10.0909090909091" customWidth="1"/>
+    <col min="10" max="10" width="9.72727272727273" customWidth="1"/>
+    <col min="11" max="13" width="8.63636363636364" customWidth="1"/>
+    <col min="14" max="14" width="12.7272727272727" customWidth="1"/>
+    <col min="15" max="15" width="21.1818181818182" customWidth="1"/>
+    <col min="16" max="16" width="8.63636363636364" customWidth="1"/>
+    <col min="17" max="17" width="12.2727272727273" customWidth="1"/>
+    <col min="18" max="18" width="26.2727272727273" customWidth="1"/>
+    <col min="19" max="19" width="19.7272727272727" customWidth="1"/>
+    <col min="20" max="20" width="15.5454545454545" customWidth="1"/>
+    <col min="21" max="21" width="14.8181818181818" customWidth="1"/>
+    <col min="22" max="22" width="18.7272727272727" customWidth="1"/>
+    <col min="23" max="23" width="21.1818181818182" customWidth="1"/>
+    <col min="24" max="24" width="32.2727272727273" customWidth="1"/>
+    <col min="25" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -1036,166 +1710,168 @@
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="P2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="Q2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="R2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="S2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="10" t="s">
+      <c r="T2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="U2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="10" t="s">
+      <c r="V2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="10" t="s">
+      <c r="W2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="10" t="s">
+      <c r="X2" s="11" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10" t="s">
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="Q3" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="R3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="S3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="T3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="U3" s="10" t="s">
+      <c r="U3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="10" t="s">
+      <c r="V3" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="W3" s="10" t="s">
+      <c r="W3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="10" t="s">
+      <c r="X3" s="11" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="G2 F10 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="32.26953125" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" customWidth="1"/>
-    <col min="5" max="7" width="8.6328125" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" customWidth="1"/>
-    <col min="9" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="9.72727272727273" customWidth="1"/>
+    <col min="2" max="2" width="12.4545454545455" customWidth="1"/>
+    <col min="3" max="3" width="32.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="12.5454545454545" customWidth="1"/>
+    <col min="5" max="7" width="8.63636363636364" customWidth="1"/>
+    <col min="8" max="8" width="17.7272727272727" customWidth="1"/>
+    <col min="9" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1224,82 +1900,84 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.5">
-      <c r="A2" s="10" t="s">
+    <row r="2" ht="15.5" spans="1:8">
+      <c r="A2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="26">
         <v>9888882626</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="27" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.5">
-      <c r="A3" s="10" t="s">
+    <row r="3" ht="15.5" spans="1:8">
+      <c r="A3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="26">
         <v>9888882626</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20" t="s">
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="27" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="H2" r:id="rId1" display="w@maxbupa.com"/>
+    <hyperlink ref="H3" r:id="rId1" display="w@maxbupa.com"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="G2 F10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" customWidth="1"/>
-    <col min="2" max="2" width="27.54296875" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" customWidth="1"/>
-    <col min="5" max="5" width="29.7265625" customWidth="1"/>
-    <col min="6" max="6" width="8.6328125" customWidth="1"/>
-    <col min="7" max="7" width="45.54296875" customWidth="1"/>
-    <col min="8" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="13.2727272727273" customWidth="1"/>
+    <col min="2" max="2" width="27.5454545454545" customWidth="1"/>
+    <col min="3" max="3" width="12.4545454545455" customWidth="1"/>
+    <col min="4" max="4" width="12.7272727272727" customWidth="1"/>
+    <col min="5" max="5" width="29.7272727272727" customWidth="1"/>
+    <col min="6" max="6" width="8.63636363636364" customWidth="1"/>
+    <col min="7" max="7" width="45.5454545454545" customWidth="1"/>
+    <col min="8" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1326,141 +2004,145 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="11" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="11" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="D3" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="E3" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.amazon.in/"/>
+    <hyperlink ref="D2" r:id="rId2" display="Damco@124"/>
+    <hyperlink ref="E2" r:id="rId3" display="XYZTestr@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.amazon.in/"/>
+    <hyperlink ref="D3" r:id="rId2" display="Damco@123"/>
+    <hyperlink ref="E3" r:id="rId3" display="XYZTestr@gmail.com"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="G2 F10 C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" customWidth="1"/>
-    <col min="2" max="3" width="15.26953125" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" customWidth="1"/>
-    <col min="6" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="14.8181818181818" customWidth="1"/>
+    <col min="2" max="3" width="15.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="27.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="16.5454545454545" customWidth="1"/>
+    <col min="6" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="25" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="11" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1469,7 +2151,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1478,31 +2160,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="G2 F10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" customWidth="1"/>
-    <col min="2" max="2" width="38.7265625" customWidth="1"/>
+    <col min="1" max="1" width="9.72727272727273" customWidth="1"/>
+    <col min="2" max="2" width="38.7272727272727" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" customWidth="1"/>
+    <col min="4" max="4" width="9.45454545454546" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="16.90625" customWidth="1"/>
-    <col min="9" max="9" width="16.1796875" customWidth="1"/>
-    <col min="10" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="7" max="7" width="16.7272727272727" customWidth="1"/>
+    <col min="8" max="8" width="16.9090909090909" customWidth="1"/>
+    <col min="9" max="9" width="16.1818181818182" customWidth="1"/>
+    <col min="10" max="1025" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1520,78 +2204,86 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="C3" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="D3" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://release.getcheddarup.com/login/"/>
+    <hyperlink ref="C2" r:id="rId2" display="sarahsmith@example.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="tester1"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://release.getcheddarup.com/login/"/>
+    <hyperlink ref="C3" r:id="rId2" display="sarahsmith@example.com"/>
+    <hyperlink ref="D3" r:id="rId3" display="tester123"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:U10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:AB10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" customWidth="1"/>
-    <col min="2" max="2" width="19.26953125" customWidth="1"/>
-    <col min="3" max="3" width="51.26953125" customWidth="1"/>
-    <col min="4" max="4" width="30.7265625" customWidth="1"/>
-    <col min="5" max="6" width="21.81640625" customWidth="1"/>
-    <col min="7" max="7" width="11.90625" customWidth="1"/>
-    <col min="8" max="8" width="18.453125" customWidth="1"/>
-    <col min="9" max="12" width="20.81640625" customWidth="1"/>
+    <col min="1" max="1" width="20.5454545454545" customWidth="1"/>
+    <col min="2" max="2" width="19.2727272727273" customWidth="1"/>
+    <col min="3" max="3" width="51.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="30.7272727272727" customWidth="1"/>
+    <col min="5" max="6" width="21.8181818181818" customWidth="1"/>
+    <col min="7" max="7" width="11.9090909090909" customWidth="1"/>
+    <col min="8" max="8" width="18.4545454545455" customWidth="1"/>
+    <col min="9" max="12" width="20.8181818181818" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="11.54296875" hidden="1"/>
+    <col min="14" max="14" width="11.5454545454545" hidden="1"/>
     <col min="15" max="15" width="9" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="17" max="17" width="14.90625" customWidth="1"/>
+    <col min="17" max="17" width="14.9090909090909" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
-    <col min="19" max="19" width="18.54296875" customWidth="1"/>
-    <col min="20" max="20" width="10.81640625" customWidth="1"/>
-    <col min="21" max="21" width="10.36328125" customWidth="1"/>
-    <col min="22" max="1031" width="8.6328125" customWidth="1"/>
+    <col min="19" max="19" width="18.5454545454545" customWidth="1"/>
+    <col min="20" max="20" width="10.8181818181818" customWidth="1"/>
+    <col min="21" max="21" width="10.3636363636364" customWidth="1"/>
+    <col min="22" max="22" width="18.8181818181818" customWidth="1"/>
+    <col min="23" max="23" width="17.3636363636364" customWidth="1"/>
+    <col min="24" max="24" width="15.9090909090909" customWidth="1"/>
+    <col min="25" max="25" width="14.7272727272727" customWidth="1"/>
+    <col min="26" max="27" width="16.9090909090909" customWidth="1"/>
+    <col min="28" max="28" width="20.6363636363636" customWidth="1"/>
+    <col min="29" max="1031" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1628,182 +2320,206 @@
       <c r="L1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="12"/>
+      <c r="N1" s="13"/>
       <c r="O1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="13" t="s">
         <v>100</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="18" t="s">
         <v>104</v>
       </c>
+      <c r="V1" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="X1" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y1" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z1" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA1" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB1" s="18" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:28">
       <c r="A2" s="4" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F2" s="7">
+        <v>116</v>
+      </c>
+      <c r="F2" s="8">
         <v>9717254315</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="J2" s="13">
+      <c r="I2" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="14">
         <v>2345</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="N2" s="14"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="U2" s="4" t="s">
+      <c r="K2" s="10" t="s">
         <v>119</v>
       </c>
+      <c r="L2" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="N2" s="15"/>
+      <c r="O2" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="V2" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="W2" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="X2" s="21">
+        <v>8745327890</v>
+      </c>
+      <c r="Y2" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z2" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA2" s="22">
+        <v>9563214467</v>
+      </c>
+      <c r="AB2" s="19" t="s">
+        <v>132</v>
+      </c>
     </row>
-    <row r="3" spans="1:21">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:28">
+      <c r="A3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" s="10">
-        <v>2000</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="P3" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
+      <c r="P3" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="19"/>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="19"/>
+      <c r="AB3" s="19"/>
     </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="J4" s="10">
-        <v>3000</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
+    <row r="9" spans="27:27">
+      <c r="AA9" s="18"/>
     </row>
-    <row r="10" spans="1:21">
-      <c r="U10" s="10"/>
+    <row r="10" spans="21:21">
+      <c r="U10" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{22CA66F3-0571-4BA4-AC8E-057A790A013A}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{9CAA5FC9-3B01-4D87-B383-6C1D2C5993B5}"/>
+    <hyperlink ref="M2" r:id="rId1" display="demo@yahooo.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="https://testingxperts-5d-dev-ed.develop.my.salesforce.com" tooltip="https://testingxperts-5d-dev-ed.develop.my.salesforce.com"/>
+    <hyperlink ref="C3" r:id="rId3" display="https://testingxperts61-dev-ed.develop.my.salesforce.com"/>
+    <hyperlink ref="E3" r:id="rId4" display="Sharma@123#&amp;"/>
+    <hyperlink ref="D2" r:id="rId5" display="xperttesting3@gmail.com" tooltip="mailto:xperttesting3@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId6" display="Tiger@2024"/>
+    <hyperlink ref="W2" r:id="rId7" display="ns123@gmail.com "/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1813,5 +2529,6 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Billing test case scenario:  Create Customer Account, Create Contact link existing /New Account
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitu Yadav\OneDrive\Documents\Selenium Project\SalesforceAutomation\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13BA69B-6E12-4BEA-8A6A-B06F3119B377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11440" tabRatio="500" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WebTestData" sheetId="1" r:id="rId1"/>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="150">
   <si>
     <t>TestData</t>
   </si>
@@ -432,31 +438,57 @@
   </si>
   <si>
     <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>ContactLastname1</t>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+  <si>
+    <t>ContactEmail1</t>
+  </si>
+  <si>
+    <t>ContactPhone1</t>
+  </si>
+  <si>
+    <t>ns123@gmail.com</t>
+  </si>
+  <si>
+    <t>8745327890</t>
+  </si>
+  <si>
+    <t>AccountName1</t>
+  </si>
+  <si>
+    <t>NishuTX</t>
+  </si>
+  <si>
+    <t>Salutation1</t>
+  </si>
+  <si>
+    <t>ContactLastName2</t>
+  </si>
+  <si>
+    <t>ContactPhone2</t>
+  </si>
+  <si>
+    <t>9563214467</t>
+  </si>
+  <si>
+    <t>Ms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="26">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -493,147 +525,16 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -654,7 +555,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -664,188 +565,8 @@
         <bgColor rgb="FF95B3D7"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -915,335 +636,60 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="48" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="48" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="48" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="48" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="48" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1316,6 +762,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1573,42 +1022,42 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="G2 F10 A1"/>
+      <selection sqref="G2 F10 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.8203125" customWidth="1"/>
-    <col min="2" max="3" width="15.2734375" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" customWidth="1"/>
-    <col min="6" max="6" width="10.8203125" customWidth="1"/>
-    <col min="7" max="7" width="28.1796875" customWidth="1"/>
-    <col min="8" max="8" width="26.2734375" customWidth="1"/>
-    <col min="9" max="9" width="10.09375" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" customWidth="1"/>
-    <col min="11" max="13" width="8.6328125" customWidth="1"/>
-    <col min="14" max="14" width="12.7265625" customWidth="1"/>
-    <col min="15" max="15" width="21.1796875" customWidth="1"/>
-    <col min="16" max="16" width="8.6328125" customWidth="1"/>
-    <col min="17" max="17" width="12.2734375" customWidth="1"/>
-    <col min="18" max="18" width="26.2734375" customWidth="1"/>
-    <col min="19" max="19" width="19.7265625" customWidth="1"/>
-    <col min="20" max="20" width="15.546875" customWidth="1"/>
-    <col min="21" max="21" width="14.8203125" customWidth="1"/>
-    <col min="22" max="22" width="18.7265625" customWidth="1"/>
-    <col min="23" max="23" width="21.1796875" customWidth="1"/>
-    <col min="24" max="24" width="32.2734375" customWidth="1"/>
-    <col min="25" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="13" width="8.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" customWidth="1"/>
+    <col min="15" max="15" width="21.140625" customWidth="1"/>
+    <col min="16" max="16" width="8.5703125" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" customWidth="1"/>
+    <col min="18" max="18" width="26.28515625" customWidth="1"/>
+    <col min="19" max="19" width="19.7109375" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" customWidth="1"/>
+    <col min="21" max="21" width="14.85546875" customWidth="1"/>
+    <col min="22" max="22" width="18.7109375" customWidth="1"/>
+    <col min="23" max="23" width="21.140625" customWidth="1"/>
+    <col min="24" max="24" width="32.28515625" customWidth="1"/>
+    <col min="25" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -1686,168 +1135,166 @@
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="V2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="W2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="X2" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6" t="s">
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="X3" s="4" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="G2 F10 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="32.2734375" customWidth="1"/>
-    <col min="4" max="4" width="12.546875" customWidth="1"/>
-    <col min="5" max="7" width="8.6328125" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" customWidth="1"/>
-    <col min="9" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="7" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1876,84 +1323,82 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" ht="14.8" spans="1:8">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:8" ht="15.75">
+      <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="15">
         <v>9888882626</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" ht="14.8" spans="1:8">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:8" ht="15.75">
+      <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="15">
         <v>9888882626</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="16" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="w@maxbupa.com"/>
-    <hyperlink ref="H3" r:id="rId1" display="w@maxbupa.com"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="G2 F10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.2734375" customWidth="1"/>
-    <col min="2" max="2" width="27.546875" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" customWidth="1"/>
-    <col min="5" max="5" width="29.7265625" customWidth="1"/>
-    <col min="6" max="6" width="8.6328125" customWidth="1"/>
-    <col min="7" max="7" width="45.546875" customWidth="1"/>
-    <col min="8" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="45.5703125" customWidth="1"/>
+    <col min="8" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1980,154 +1425,150 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.amazon.in/"/>
-    <hyperlink ref="D2" r:id="rId2" display="Damco@124"/>
-    <hyperlink ref="E2" r:id="rId3" display="XYZTestr@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.amazon.in/"/>
-    <hyperlink ref="D3" r:id="rId2" display="Damco@123"/>
-    <hyperlink ref="E3" r:id="rId3" display="XYZTestr@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="D3" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="E3" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="G2 F10 C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.8203125" customWidth="1"/>
-    <col min="2" max="3" width="15.2734375" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.546875" customWidth="1"/>
-    <col min="6" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="14" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="G2 F10 C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2136,33 +1577,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="G2 F10 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" customWidth="1"/>
-    <col min="2" max="2" width="38.7265625" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="16.90625" customWidth="1"/>
-    <col min="9" max="9" width="16.1796875" customWidth="1"/>
-    <col min="10" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="10" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2180,88 +1619,93 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://release.getcheddarup.com/login/"/>
-    <hyperlink ref="C2" r:id="rId2" display="sarahsmith@example.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="tester1"/>
-    <hyperlink ref="B3" r:id="rId1" display="https://release.getcheddarup.com/login/"/>
-    <hyperlink ref="C3" r:id="rId2" display="sarahsmith@example.com"/>
-    <hyperlink ref="D3" r:id="rId3" display="tester123"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="D3" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:AA7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.546875" customWidth="1"/>
-    <col min="2" max="2" width="19.2734375" customWidth="1"/>
-    <col min="3" max="3" width="51.2734375" customWidth="1"/>
-    <col min="4" max="4" width="30.7265625" customWidth="1"/>
-    <col min="5" max="6" width="21.8203125" customWidth="1"/>
-    <col min="7" max="7" width="11.90625" customWidth="1"/>
-    <col min="8" max="8" width="18.453125" customWidth="1"/>
-    <col min="9" max="12" width="20.8203125" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="51.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="12" width="20.85546875" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
     <col min="14" max="14" width="9" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
-    <col min="16" max="16" width="14.90625" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" customWidth="1"/>
     <col min="17" max="17" width="16" customWidth="1"/>
-    <col min="18" max="18" width="18.546875" customWidth="1"/>
-    <col min="19" max="19" width="10.8203125" customWidth="1"/>
-    <col min="20" max="20" width="10.3671875" customWidth="1"/>
-    <col min="21" max="23" width="8.6328125" customWidth="1"/>
-    <col min="24" max="24" width="11.328125" customWidth="1"/>
-    <col min="25" max="25" width="8.6328125" customWidth="1"/>
-    <col min="26" max="26" width="15.1015625" customWidth="1"/>
-    <col min="27" max="27" width="10.28125" customWidth="1"/>
-    <col min="28" max="1029" width="8.6328125" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" customWidth="1"/>
+    <col min="19" max="19" width="10.85546875" customWidth="1"/>
+    <col min="20" max="20" width="10.42578125" customWidth="1"/>
+    <col min="21" max="23" width="8.5703125" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" customWidth="1"/>
+    <col min="25" max="25" width="8.5703125" customWidth="1"/>
+    <col min="26" max="26" width="15.140625" customWidth="1"/>
+    <col min="27" max="27" width="10.28515625" customWidth="1"/>
+    <col min="28" max="28" width="17.42578125" customWidth="1"/>
+    <col min="29" max="29" width="24.28515625" customWidth="1"/>
+    <col min="30" max="30" width="14.5703125" customWidth="1"/>
+    <col min="31" max="31" width="16.140625" customWidth="1"/>
+    <col min="32" max="32" width="12.85546875" customWidth="1"/>
+    <col min="33" max="33" width="17.5703125" customWidth="1"/>
+    <col min="34" max="34" width="17.140625" customWidth="1"/>
+    <col min="35" max="1029" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:34">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>90</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2273,223 +1717,263 @@
       <c r="E1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="T1" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="U1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="V1" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="W1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="X1" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Y1" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="Z1" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="AA1" s="16" t="s">
+      <c r="AA1" s="11" t="s">
         <v>109</v>
       </c>
+      <c r="AB1" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC1" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD1" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE1" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF1" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG1" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH1" s="29" t="s">
+        <v>146</v>
+      </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:34">
       <c r="A2" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="3">
         <v>9717254315</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="12">
+      <c r="J2" s="8">
         <v>2345</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11" t="s">
+      <c r="O2" s="7"/>
+      <c r="P2" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="Q2" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="R2" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="S2" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="T2" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="U2" s="11" t="s">
+      <c r="U2" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="V2" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="W2" s="11" t="s">
+      <c r="W2" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="X2" s="11" t="s">
+      <c r="X2" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="Y2" s="11" t="s">
+      <c r="Y2" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="Z2" s="11" t="s">
+      <c r="Z2" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="AA2" s="11" t="s">
+      <c r="AA2" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="AB2" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC2" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD2" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE2" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="AG2" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="AH2" s="4" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="3" spans="1:27">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:34">
+      <c r="A3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="15" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4"/>
     </row>
-    <row r="7" spans="20:20">
-      <c r="T7" s="6"/>
+    <row r="7" spans="1:34">
+      <c r="T7" s="28"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" display="demo@yahooo.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="https://testingxperts-5d-dev-ed.develop.my.salesforce.com"/>
-    <hyperlink ref="C3" r:id="rId3" display="https://testingxperts61-dev-ed.develop.my.salesforce.com"/>
-    <hyperlink ref="E3" r:id="rId4" display="Sharma@123#&amp;"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commited the changes and add product in marketing crm
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -390,7 +390,7 @@
     <t>Mr</t>
   </si>
   <si>
-    <t>DemoOpportunity</t>
+    <t>DemoOpportunity1</t>
   </si>
   <si>
     <t>Prospecting</t>
@@ -1183,7 +1183,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1203,8 +1203,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1722,7 +1720,7 @@
       <c r="D2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="21" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="11" t="s">
@@ -1796,7 +1794,7 @@
       <c r="D3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="21" t="s">
         <v>27</v>
       </c>
       <c r="F3" s="11" t="s">
@@ -1904,25 +1902,25 @@
       <c r="A2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="24">
         <v>9888882626</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="25" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1930,21 +1928,21 @@
       <c r="A3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="24">
         <v>9888882626</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="25" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2007,7 +2005,7 @@
       <c r="A2" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>63</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -2016,7 +2014,7 @@
       <c r="D2" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="21" t="s">
         <v>66</v>
       </c>
       <c r="F2" s="11" t="s">
@@ -2030,7 +2028,7 @@
       <c r="A3" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="21" t="s">
         <v>63</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -2039,7 +2037,7 @@
       <c r="D3" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="21" t="s">
         <v>66</v>
       </c>
       <c r="F3" s="11" t="s">
@@ -2083,19 +2081,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="23" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2207,10 +2205,10 @@
       <c r="A2" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="21" t="s">
         <v>86</v>
       </c>
       <c r="D2" s="11" t="s">
@@ -2221,10 +2219,10 @@
       <c r="A3" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="21" t="s">
         <v>86</v>
       </c>
       <c r="D3" s="11" t="s">
@@ -2251,8 +2249,8 @@
   <sheetPr/>
   <dimension ref="A1:AB10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -2429,25 +2427,25 @@
       <c r="U2" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="V2" s="19" t="s">
+      <c r="V2" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="W2" s="20" t="s">
+      <c r="W2" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="X2" s="21">
+      <c r="X2" s="19">
         <v>8745327890</v>
       </c>
-      <c r="Y2" s="19" t="s">
+      <c r="Y2" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="Z2" s="19" t="s">
+      <c r="Z2" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="AA2" s="22">
+      <c r="AA2" s="20">
         <v>9563214467</v>
       </c>
-      <c r="AB2" s="19" t="s">
+      <c r="AB2" s="11" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2487,13 +2485,13 @@
       <c r="U3" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="V3" s="19"/>
-      <c r="W3" s="19"/>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="19"/>
-      <c r="Z3" s="19"/>
-      <c r="AA3" s="19"/>
-      <c r="AB3" s="19"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
     </row>
     <row r="9" spans="27:27">
       <c r="AA9" s="18"/>

</xml_diff>

<commit_message>
Create new case flows in billing
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="156">
   <si>
     <t>TestData</t>
   </si>
@@ -309,6 +309,9 @@
     <t>AccountName</t>
   </si>
   <si>
+    <t>PaymentsAccount</t>
+  </si>
+  <si>
     <t>Phone</t>
   </si>
   <si>
@@ -372,12 +375,45 @@
     <t>ContactLastName2</t>
   </si>
   <si>
+    <t>InReviewStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ApprovedStatus </t>
+  </si>
+  <si>
+    <t>changeStatusAsDraft</t>
+  </si>
+  <si>
+    <t>InvoiceNumber</t>
+  </si>
+  <si>
+    <t>TaxStatus</t>
+  </si>
+  <si>
+    <t>PostedStatus</t>
+  </si>
+  <si>
+    <t>PaymentType</t>
+  </si>
+  <si>
+    <t>CaseOrigin</t>
+  </si>
+  <si>
+    <t>EditCaseOrigin</t>
+  </si>
+  <si>
+    <t>WebCompany</t>
+  </si>
+  <si>
     <t>TestData1</t>
   </si>
   <si>
     <t>TXTest</t>
   </si>
   <si>
+    <t>Billing Account</t>
+  </si>
+  <si>
     <t>https://testingxperts-5d-dev-ed.develop.my.salesforce.com</t>
   </si>
   <si>
@@ -433,6 +469,27 @@
   </si>
   <si>
     <t>Sharma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Review </t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>Draft</t>
+  </si>
+  <si>
+    <t>INV-0005</t>
+  </si>
+  <si>
+    <t>Posted</t>
+  </si>
+  <si>
+    <t>Credit Card</t>
+  </si>
+  <si>
+    <t>TestingXperts</t>
   </si>
   <si>
     <t>https://testingxperts61-dev-ed.develop.my.salesforce.com</t>
@@ -1183,21 +1240,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="6" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="6" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -1205,9 +1262,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1708,140 +1762,140 @@
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="P2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="Q2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="R2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="S2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="T2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="11" t="s">
+      <c r="U2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="V2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="11" t="s">
+      <c r="W2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="11" t="s">
+      <c r="X2" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11" t="s">
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="R3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="S3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="T3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="U3" s="11" t="s">
+      <c r="U3" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="11" t="s">
+      <c r="V3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="W3" s="11" t="s">
+      <c r="W3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="X3" s="11" t="s">
+      <c r="X3" s="9" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1899,50 +1953,50 @@
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:8">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>9888882626</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="24" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" ht="15.5" spans="1:8">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>9888882626</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="24" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2002,48 +2056,48 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="9" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="9" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2081,53 +2135,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2202,30 +2256,30 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2247,41 +2301,46 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AB10"/>
+  <dimension ref="A1:AM10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="20.5454545454545" customWidth="1"/>
     <col min="2" max="2" width="19.2727272727273" customWidth="1"/>
-    <col min="3" max="3" width="51.2727272727273" customWidth="1"/>
-    <col min="4" max="4" width="30.7272727272727" customWidth="1"/>
-    <col min="5" max="6" width="21.8181818181818" customWidth="1"/>
-    <col min="7" max="7" width="11.9090909090909" customWidth="1"/>
-    <col min="8" max="8" width="18.4545454545455" customWidth="1"/>
-    <col min="9" max="12" width="20.8181818181818" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="11.5454545454545" hidden="1"/>
-    <col min="15" max="15" width="9" customWidth="1"/>
-    <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="17" max="17" width="14.9090909090909" customWidth="1"/>
-    <col min="18" max="18" width="16" customWidth="1"/>
-    <col min="19" max="19" width="18.5454545454545" customWidth="1"/>
-    <col min="20" max="20" width="10.8181818181818" customWidth="1"/>
-    <col min="21" max="21" width="10.3636363636364" customWidth="1"/>
-    <col min="22" max="22" width="18.8181818181818" customWidth="1"/>
-    <col min="23" max="23" width="17.3636363636364" customWidth="1"/>
-    <col min="24" max="24" width="15.9090909090909" customWidth="1"/>
-    <col min="25" max="25" width="14.7272727272727" customWidth="1"/>
-    <col min="26" max="27" width="16.9090909090909" customWidth="1"/>
-    <col min="28" max="28" width="20.6363636363636" customWidth="1"/>
-    <col min="29" max="1031" width="8.63636363636364" customWidth="1"/>
+    <col min="3" max="4" width="51.2727272727273" customWidth="1"/>
+    <col min="5" max="5" width="30.7272727272727" customWidth="1"/>
+    <col min="6" max="7" width="21.8181818181818" customWidth="1"/>
+    <col min="8" max="8" width="11.9090909090909" customWidth="1"/>
+    <col min="9" max="9" width="18.4545454545455" customWidth="1"/>
+    <col min="10" max="13" width="20.8181818181818" customWidth="1"/>
+    <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="11.5454545454545" hidden="1"/>
+    <col min="16" max="16" width="9" customWidth="1"/>
+    <col min="17" max="17" width="10" customWidth="1"/>
+    <col min="18" max="18" width="14.9090909090909" customWidth="1"/>
+    <col min="19" max="19" width="16" customWidth="1"/>
+    <col min="20" max="20" width="18.5454545454545" customWidth="1"/>
+    <col min="21" max="21" width="10.8181818181818" customWidth="1"/>
+    <col min="22" max="22" width="10.3636363636364" customWidth="1"/>
+    <col min="23" max="23" width="18.8181818181818" customWidth="1"/>
+    <col min="24" max="24" width="17.3636363636364" customWidth="1"/>
+    <col min="25" max="25" width="15.9090909090909" customWidth="1"/>
+    <col min="26" max="26" width="14.7272727272727" customWidth="1"/>
+    <col min="27" max="28" width="16.9090909090909" customWidth="1"/>
+    <col min="29" max="32" width="20.6363636363636" customWidth="1"/>
+    <col min="33" max="33" width="14.9090909090909" customWidth="1"/>
+    <col min="34" max="35" width="8.63636363636364" customWidth="1"/>
+    <col min="36" max="36" width="17.1818181818182" customWidth="1"/>
+    <col min="37" max="38" width="8.63636363636364" customWidth="1"/>
+    <col min="39" max="39" width="16" customWidth="1"/>
+    <col min="40" max="1036" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:39">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2289,58 +2348,58 @@
         <v>90</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="3" t="s">
+      <c r="N1" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="O1" s="12"/>
+      <c r="P1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="T1" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="U1" s="12" t="s">
         <v>104</v>
       </c>
       <c r="V1" s="18" t="s">
@@ -2364,150 +2423,220 @@
       <c r="AB1" s="18" t="s">
         <v>111</v>
       </c>
+      <c r="AC1" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI1" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ1" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK1" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL1" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM1" s="12" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="2" spans="1:28">
-      <c r="A2" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F2" s="8">
+    <row r="2" spans="1:39">
+      <c r="A2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="7">
         <v>9717254315</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="J2" s="14">
+      <c r="J2" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="K2" s="14">
         <v>2345</v>
       </c>
-      <c r="K2" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="N2" s="15"/>
-      <c r="O2" s="16" t="s">
-        <v>122</v>
-      </c>
+      <c r="L2" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="O2" s="15"/>
       <c r="P2" s="16" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="Q2" s="16" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="R2" s="16" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="S2" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="V2" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="X2" s="19">
+        <v>137</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y2" s="19">
         <v>8745327890</v>
       </c>
-      <c r="Y2" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="Z2" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="AA2" s="20">
+      <c r="Z2" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB2" s="9">
         <v>9563214467</v>
       </c>
-      <c r="AB2" s="11" t="s">
-        <v>132</v>
+      <c r="AC2" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE2" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="AF2" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="AG2" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI2" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM2" s="9" t="s">
+        <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:32">
+      <c r="A3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="P3" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q3" s="17"/>
+      <c r="Q3" s="17" t="s">
+        <v>155</v>
+      </c>
       <c r="R3" s="17"/>
       <c r="S3" s="17"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="11"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9"/>
     </row>
-    <row r="9" spans="27:27">
-      <c r="AA9" s="18"/>
+    <row r="9" spans="28:28">
+      <c r="AB9" s="18"/>
     </row>
-    <row r="10" spans="21:21">
-      <c r="U10" s="11"/>
+    <row r="10" spans="22:22">
+      <c r="V10" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" display="demo@yahooo.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="https://testingxperts-5d-dev-ed.develop.my.salesforce.com" tooltip="https://testingxperts-5d-dev-ed.develop.my.salesforce.com"/>
-    <hyperlink ref="C3" r:id="rId3" display="https://testingxperts61-dev-ed.develop.my.salesforce.com"/>
-    <hyperlink ref="E3" r:id="rId4" display="Sharma@123#&amp;"/>
-    <hyperlink ref="D2" r:id="rId5" display="xperttesting3@gmail.com" tooltip="mailto:xperttesting3@gmail.com"/>
-    <hyperlink ref="E2" r:id="rId6" display="Tiger@2024"/>
-    <hyperlink ref="W2" r:id="rId7" display="ns123@gmail.com "/>
+    <hyperlink ref="N2" r:id="rId1" display="demo@yahooo.com"/>
+    <hyperlink ref="D2" r:id="rId2" display="https://testingxperts-5d-dev-ed.develop.my.salesforce.com" tooltip="https://testingxperts-5d-dev-ed.develop.my.salesforce.com"/>
+    <hyperlink ref="D3" r:id="rId3" display="https://testingxperts61-dev-ed.develop.my.salesforce.com"/>
+    <hyperlink ref="F3" r:id="rId4" display="Sharma@123#&amp;"/>
+    <hyperlink ref="E2" r:id="rId5" display="xperttesting3@gmail.com" tooltip="mailto:xperttesting3@gmail.com"/>
+    <hyperlink ref="F2" r:id="rId6" display="Tiger@2024"/>
+    <hyperlink ref="X2" r:id="rId7" display="ns123@gmail.com "/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Refactoring and code enhancements
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Salesforce" sheetId="7" r:id="rId7"/>
     <sheet name="SalesforceLogin" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="182">
   <si>
     <t>TestData</t>
   </si>
@@ -405,6 +405,54 @@
     <t>WebCompany</t>
   </si>
   <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>CaseNumber</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>NewDiscount</t>
+  </si>
+  <si>
+    <t>NewProductName</t>
+  </si>
+  <si>
+    <t>searchProduct</t>
+  </si>
+  <si>
+    <t>roleValue</t>
+  </si>
+  <si>
+    <t>actionValue</t>
+  </si>
+  <si>
+    <t>quoteValue</t>
+  </si>
+  <si>
+    <t>ProductName_new</t>
+  </si>
+  <si>
+    <t>ProductCode</t>
+  </si>
+  <si>
+    <t>ProductFamily</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>sku</t>
+  </si>
+  <si>
     <t>TestData1</t>
   </si>
   <si>
@@ -490,6 +538,36 @@
   </si>
   <si>
     <t>TestingXperts</t>
+  </si>
+  <si>
+    <t>2FAUSBKEY</t>
+  </si>
+  <si>
+    <t>Anjali</t>
+  </si>
+  <si>
+    <t>00001058</t>
+  </si>
+  <si>
+    <t>PANEL-BUY</t>
+  </si>
+  <si>
+    <t>INTP</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>Assign</t>
+  </si>
+  <si>
+    <t>IntelPro</t>
+  </si>
+  <si>
+    <t>Hardware Family selected</t>
+  </si>
+  <si>
+    <t>samsung</t>
   </si>
   <si>
     <t>https://testingxperts61-dev-ed.develop.my.salesforce.com</t>
@@ -1240,7 +1318,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1263,11 +1341,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1774,7 +1854,7 @@
       <c r="D2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="21" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="9" t="s">
@@ -1848,7 +1928,7 @@
       <c r="D3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="21" t="s">
         <v>27</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -1956,25 +2036,25 @@
       <c r="A2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="24">
         <v>9888882626</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="25" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1982,21 +2062,21 @@
       <c r="A3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="24">
         <v>9888882626</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="25" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2059,7 +2139,7 @@
       <c r="A2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>63</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -2068,7 +2148,7 @@
       <c r="D2" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="21" t="s">
         <v>66</v>
       </c>
       <c r="F2" s="9" t="s">
@@ -2082,7 +2162,7 @@
       <c r="A3" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>63</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -2091,7 +2171,7 @@
       <c r="D3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="21" t="s">
         <v>66</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -2135,19 +2215,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="23" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2259,10 +2339,10 @@
       <c r="A2" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="21" t="s">
         <v>86</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -2273,10 +2353,10 @@
       <c r="A3" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>86</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -2301,10 +2381,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AM10"/>
+  <dimension ref="A1:BC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AM2" sqref="AM2"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="BC2" sqref="BC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -2337,10 +2417,24 @@
     <col min="36" max="36" width="17.1818181818182" customWidth="1"/>
     <col min="37" max="38" width="8.63636363636364" customWidth="1"/>
     <col min="39" max="39" width="16" customWidth="1"/>
-    <col min="40" max="1036" width="8.63636363636364" customWidth="1"/>
+    <col min="40" max="40" width="13.0909090909091" customWidth="1"/>
+    <col min="41" max="41" width="16.5454545454545" customWidth="1"/>
+    <col min="42" max="42" width="18.8181818181818" customWidth="1"/>
+    <col min="43" max="43" width="20.0909090909091" customWidth="1"/>
+    <col min="44" max="44" width="8.63636363636364" customWidth="1"/>
+    <col min="45" max="45" width="15.5454545454545" customWidth="1"/>
+    <col min="46" max="46" width="17.0909090909091" customWidth="1"/>
+    <col min="47" max="47" width="17.6363636363636" customWidth="1"/>
+    <col min="48" max="48" width="16.0909090909091" customWidth="1"/>
+    <col min="49" max="49" width="21.7272727272727" customWidth="1"/>
+    <col min="50" max="50" width="19.4545454545455" customWidth="1"/>
+    <col min="51" max="51" width="20.9090909090909" customWidth="1"/>
+    <col min="52" max="52" width="18.1818181818182" customWidth="1"/>
+    <col min="53" max="53" width="30.1818181818182" customWidth="1"/>
+    <col min="54" max="1035" width="8.63636363636364" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:55">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2456,113 +2550,161 @@
       <c r="AM1" s="12" t="s">
         <v>122</v>
       </c>
+      <c r="AN1" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="AO1" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP1" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="AQ1" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="AR1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS1" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="AT1" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="AU1" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="AV1" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="AW1" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="AX1" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="AY1" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="AZ1" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="BA1" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="BB1" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="BC1" s="12" t="s">
+        <v>138</v>
+      </c>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:55">
       <c r="A2" s="3" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="G2" s="7">
         <v>9717254315</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>54</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="K2" s="14">
         <v>2345</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="N2" s="15" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="O2" s="15"/>
       <c r="P2" s="16" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="Q2" s="16" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="R2" s="16" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="S2" s="16" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="T2" s="16" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="W2" s="9" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="Y2" s="19">
         <v>8745327890</v>
       </c>
       <c r="Z2" s="9" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="AA2" s="9" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="AB2" s="9">
         <v>9563214467</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="AD2" s="9" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="AE2" s="9" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="AF2" s="9" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="AG2" s="9" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="AH2" s="9" t="s">
         <v>30</v>
       </c>
       <c r="AI2" s="9" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="AJ2" s="9" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="AK2" s="9" t="s">
         <v>92</v>
@@ -2571,7 +2713,55 @@
         <v>22</v>
       </c>
       <c r="AM2" s="9" t="s">
-        <v>151</v>
+        <v>167</v>
+      </c>
+      <c r="AN2" s="9">
+        <v>5</v>
+      </c>
+      <c r="AO2" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="AP2" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="AQ2" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="AR2" s="9">
+        <v>10</v>
+      </c>
+      <c r="AS2" s="9">
+        <v>8</v>
+      </c>
+      <c r="AT2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="AU2" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="AV2" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="AW2" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="AX2" s="9">
+        <v>3000</v>
+      </c>
+      <c r="AY2" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="AZ2" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="BA2" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="BB2" s="20">
+        <v>2</v>
+      </c>
+      <c r="BC2" s="20" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:32">
@@ -2581,13 +2771,13 @@
       <c r="B3" s="9"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
@@ -2599,17 +2789,17 @@
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
       <c r="P3" s="17" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="Q3" s="17" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="R3" s="17"/>
       <c r="S3" s="17"/>
       <c r="T3" s="17"/>
       <c r="U3" s="9"/>
       <c r="V3" s="9" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="W3" s="9"/>
       <c r="X3" s="9"/>

</xml_diff>